<commit_message>
re-ran on updated results
</commit_message>
<xml_diff>
--- a/tables/output/TableS3-DeSeq2-sbi-SFs.xlsx
+++ b/tables/output/TableS3-DeSeq2-sbi-SFs.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t xml:space="preserve">gene</t>
   </si>
@@ -35,9 +35,6 @@
     <t xml:space="preserve">padj</t>
   </si>
   <si>
-    <t xml:space="preserve">HNRNPA1</t>
-  </si>
-  <si>
     <t xml:space="preserve">PABPC1</t>
   </si>
   <si>
@@ -53,6 +50,9 @@
     <t xml:space="preserve">HNRNPK</t>
   </si>
   <si>
+    <t xml:space="preserve">SFPQ</t>
+  </si>
+  <si>
     <t xml:space="preserve">HNRNPH1</t>
   </si>
   <si>
@@ -116,15 +116,15 @@
     <t xml:space="preserve">SRSF6</t>
   </si>
   <si>
+    <t xml:space="preserve">RBFOX2</t>
+  </si>
+  <si>
     <t xml:space="preserve">G3BP1</t>
   </si>
   <si>
     <t xml:space="preserve">CELF1</t>
   </si>
   <si>
-    <t xml:space="preserve">SRRM1</t>
-  </si>
-  <si>
     <t xml:space="preserve">TARDBP</t>
   </si>
   <si>
@@ -140,9 +140,6 @@
     <t xml:space="preserve">ZNF638</t>
   </si>
   <si>
-    <t xml:space="preserve">PABPC4</t>
-  </si>
-  <si>
     <t xml:space="preserve">CLK1</t>
   </si>
   <si>
@@ -212,6 +209,12 @@
     <t xml:space="preserve">PTBP2</t>
   </si>
   <si>
+    <t xml:space="preserve">MSI1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELAVL4</t>
+  </si>
+  <si>
     <t xml:space="preserve">KHDRBS3</t>
   </si>
   <si>
@@ -221,9 +224,6 @@
     <t xml:space="preserve">RBM15</t>
   </si>
   <si>
-    <t xml:space="preserve">RBMXL1</t>
-  </si>
-  <si>
     <t xml:space="preserve">SRRM4</t>
   </si>
   <si>
@@ -245,10 +245,16 @@
     <t xml:space="preserve">RBM41</t>
   </si>
   <si>
+    <t xml:space="preserve">WT1</t>
+  </si>
+  <si>
     <t xml:space="preserve">ZC3H10</t>
   </si>
   <si>
     <t xml:space="preserve">CELF6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RBM24</t>
   </si>
 </sst>
 </file>
@@ -608,22 +614,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>24968.6241078584</v>
+        <v>21413.9444882445</v>
       </c>
       <c r="C2" t="n">
-        <v>0.252841869572805</v>
+        <v>-0.395491771446074</v>
       </c>
       <c r="D2" t="n">
-        <v>0.108484730557055</v>
+        <v>0.111356706801239</v>
       </c>
       <c r="E2" t="n">
-        <v>2.33066781172331</v>
+        <v>-3.55157567789778</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0197708827332515</v>
+        <v>0.000382931853913751</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0423661772855389</v>
+        <v>0.00136523530525772</v>
       </c>
     </row>
     <row r="3">
@@ -631,22 +637,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>22176.5413974474</v>
+        <v>29625.9238314483</v>
       </c>
       <c r="C3" t="n">
-        <v>0.376240283613877</v>
+        <v>0.280456707214421</v>
       </c>
       <c r="D3" t="n">
-        <v>0.107055447417581</v>
+        <v>0.10989920391986</v>
       </c>
       <c r="E3" t="n">
-        <v>3.51444314782332</v>
+        <v>2.55194484774371</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00044067698898992</v>
+        <v>0.0107123474561109</v>
       </c>
       <c r="G3" t="n">
-        <v>0.00140855138871232</v>
+        <v>0.0274503903562841</v>
       </c>
     </row>
     <row r="4">
@@ -654,22 +660,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>28745.1410134979</v>
+        <v>17105.9396699372</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.26996697122499</v>
+        <v>-0.359916309398203</v>
       </c>
       <c r="D4" t="n">
-        <v>0.104429298530204</v>
+        <v>0.117419582518479</v>
       </c>
       <c r="E4" t="n">
-        <v>-2.58516503533639</v>
+        <v>-3.06521537275574</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00973323961483227</v>
+        <v>0.00217513301296727</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0228122803472631</v>
+        <v>0.00660595952086357</v>
       </c>
     </row>
     <row r="5">
@@ -677,22 +683,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>17682.291500198</v>
+        <v>17145.0455603426</v>
       </c>
       <c r="C5" t="n">
-        <v>0.304807856848774</v>
+        <v>-1.05740427150994</v>
       </c>
       <c r="D5" t="n">
-        <v>0.113175763381531</v>
+        <v>0.151913112208005</v>
       </c>
       <c r="E5" t="n">
-        <v>2.69322554353997</v>
+        <v>-6.96058593060819</v>
       </c>
       <c r="F5" t="n">
-        <v>0.00707643803543069</v>
+        <v>0.00000000000338860392151664</v>
       </c>
       <c r="G5" t="n">
-        <v>0.017401077136305</v>
+        <v>0.000000000111146208625746</v>
       </c>
     </row>
     <row r="6">
@@ -700,22 +706,22 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>18063.2470982188</v>
+        <v>17025.9790703674</v>
       </c>
       <c r="C6" t="n">
-        <v>1.13357555863104</v>
+        <v>-0.400565512875317</v>
       </c>
       <c r="D6" t="n">
-        <v>0.149876752105341</v>
+        <v>0.0955411307769207</v>
       </c>
       <c r="E6" t="n">
-        <v>7.56338486594845</v>
+        <v>-4.19259757151712</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0000000000000392713425840456</v>
+        <v>0.0000275778405771315</v>
       </c>
       <c r="G6" t="n">
-        <v>0.00000000000147267534690171</v>
+        <v>0.000137053510746956</v>
       </c>
     </row>
     <row r="7">
@@ -723,22 +729,22 @@
         <v>12</v>
       </c>
       <c r="B7" t="n">
-        <v>16868.4424658886</v>
+        <v>15331.6791294024</v>
       </c>
       <c r="C7" t="n">
-        <v>0.397778760618737</v>
+        <v>0.288425447691839</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0874240294687445</v>
+        <v>0.11601132410771</v>
       </c>
       <c r="E7" t="n">
-        <v>4.54999344042989</v>
+        <v>2.48618356794249</v>
       </c>
       <c r="F7" t="n">
-        <v>0.00000536475879581421</v>
+        <v>0.0129121342430727</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0000277487523921425</v>
+        <v>0.0317521782535866</v>
       </c>
     </row>
     <row r="8">
@@ -746,22 +752,22 @@
         <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>10694.3900643543</v>
+        <v>10965.1673681756</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.29479653441993</v>
+        <v>0.323770095545052</v>
       </c>
       <c r="D8" t="n">
-        <v>0.117656660332894</v>
+        <v>0.121795156030433</v>
       </c>
       <c r="E8" t="n">
-        <v>-2.5055660562338</v>
+        <v>2.65831668596207</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0122255559708081</v>
+        <v>0.00785320603531949</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0282128214710956</v>
+        <v>0.0211135375375803</v>
       </c>
     </row>
     <row r="9">
@@ -769,22 +775,22 @@
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>12378.2063338046</v>
+        <v>12811.145790085</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.313072621337658</v>
+        <v>0.368747547359242</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0897736597773991</v>
+        <v>0.0939940457858326</v>
       </c>
       <c r="E9" t="n">
-        <v>-3.48735500049733</v>
+        <v>3.9230947479316</v>
       </c>
       <c r="F9" t="n">
-        <v>0.000487823364562153</v>
+        <v>0.0000874187521095733</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0014933368302923</v>
+        <v>0.000377280930157106</v>
       </c>
     </row>
     <row r="10">
@@ -792,22 +798,22 @@
         <v>15</v>
       </c>
       <c r="B10" t="n">
-        <v>12014.187561198</v>
+        <v>12081.3644648276</v>
       </c>
       <c r="C10" t="n">
-        <v>0.696742222438686</v>
+        <v>-0.68018014357471</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0919280019294596</v>
+        <v>0.0912297827168843</v>
       </c>
       <c r="E10" t="n">
-        <v>7.57921642823616</v>
+        <v>-7.45568084586511</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0000000000000347648159208473</v>
+        <v>0.0000000000000894049280531944</v>
       </c>
       <c r="G10" t="n">
-        <v>0.00000000000147267534690171</v>
+        <v>0.0000000000069682117666251</v>
       </c>
     </row>
     <row r="11">
@@ -815,22 +821,22 @@
         <v>16</v>
       </c>
       <c r="B11" t="n">
-        <v>9722.35651324658</v>
+        <v>9649.38986704767</v>
       </c>
       <c r="C11" t="n">
-        <v>0.343614293529043</v>
+        <v>-0.331899210302079</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0945002680339075</v>
+        <v>0.105689379681092</v>
       </c>
       <c r="E11" t="n">
-        <v>3.63611977699102</v>
+        <v>-3.14032697801381</v>
       </c>
       <c r="F11" t="n">
-        <v>0.000276775675833371</v>
+        <v>0.00168759360998896</v>
       </c>
       <c r="G11" t="n">
-        <v>0.00101259393597574</v>
+        <v>0.00532241061611903</v>
       </c>
     </row>
     <row r="12">
@@ -838,22 +844,22 @@
         <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>7867.79320071185</v>
+        <v>8275.86662467782</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.709112346632881</v>
+        <v>0.810126221942985</v>
       </c>
       <c r="D12" t="n">
-        <v>0.121834140189358</v>
+        <v>0.122569147726487</v>
       </c>
       <c r="E12" t="n">
-        <v>-5.82030903267968</v>
+        <v>6.60954438347555</v>
       </c>
       <c r="F12" t="n">
-        <v>0.00000000587389208586055</v>
+        <v>0.000000000038550463205887</v>
       </c>
       <c r="G12" t="n">
-        <v>0.000000080098528443553</v>
+        <v>0.000000000702475107307274</v>
       </c>
     </row>
     <row r="13">
@@ -861,22 +867,22 @@
         <v>18</v>
       </c>
       <c r="B13" t="n">
-        <v>7442.06678688772</v>
+        <v>7060.39441006975</v>
       </c>
       <c r="C13" t="n">
-        <v>0.627154793638574</v>
+        <v>-0.670978616162992</v>
       </c>
       <c r="D13" t="n">
-        <v>0.157649430002562</v>
+        <v>0.173076512901772</v>
       </c>
       <c r="E13" t="n">
-        <v>3.97816087015591</v>
+        <v>-3.87677452540196</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0000694503787422546</v>
+        <v>0.000105850365725583</v>
       </c>
       <c r="G13" t="n">
-        <v>0.000267116841316364</v>
+        <v>0.000445114358435784</v>
       </c>
     </row>
     <row r="14">
@@ -884,22 +890,22 @@
         <v>19</v>
       </c>
       <c r="B14" t="n">
-        <v>7975.03946751331</v>
+        <v>8003.06222793178</v>
       </c>
       <c r="C14" t="n">
-        <v>0.373532639377811</v>
+        <v>-0.367145514669166</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0772701747292576</v>
+        <v>0.0778183001408533</v>
       </c>
       <c r="E14" t="n">
-        <v>4.83411148850912</v>
+        <v>-4.71798425312069</v>
       </c>
       <c r="F14" t="n">
-        <v>0.00000133741621581328</v>
+        <v>0.00000238192925672816</v>
       </c>
       <c r="G14" t="n">
-        <v>0.00000743009008785153</v>
+        <v>0.000014468014744571</v>
       </c>
     </row>
     <row r="15">
@@ -907,22 +913,22 @@
         <v>20</v>
       </c>
       <c r="B15" t="n">
-        <v>5928.03824796023</v>
+        <v>6144.14236279482</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.701133815761292</v>
+        <v>0.747952249287623</v>
       </c>
       <c r="D15" t="n">
-        <v>0.142717283709164</v>
+        <v>0.145393946657754</v>
       </c>
       <c r="E15" t="n">
-        <v>-4.91274635796808</v>
+        <v>5.14431492150251</v>
       </c>
       <c r="F15" t="n">
-        <v>0.000000898094285900493</v>
+        <v>0.00000026849880431317</v>
       </c>
       <c r="G15" t="n">
-        <v>0.00000585713664717713</v>
+        <v>0.00000200153654124363</v>
       </c>
     </row>
     <row r="16">
@@ -930,22 +936,22 @@
         <v>21</v>
       </c>
       <c r="B16" t="n">
-        <v>7113.30554485757</v>
+        <v>6995.87319487614</v>
       </c>
       <c r="C16" t="n">
-        <v>0.760449352847779</v>
+        <v>-0.716777030358966</v>
       </c>
       <c r="D16" t="n">
-        <v>0.148139870901126</v>
+        <v>0.154317974837913</v>
       </c>
       <c r="E16" t="n">
-        <v>5.13331993758337</v>
+        <v>-4.64480583750419</v>
       </c>
       <c r="F16" t="n">
-        <v>0.000000284675376830798</v>
+        <v>0.00000340396437982646</v>
       </c>
       <c r="G16" t="n">
-        <v>0.00000228344290384427</v>
+        <v>0.0000199375056532693</v>
       </c>
     </row>
     <row r="17">
@@ -953,22 +959,22 @@
         <v>22</v>
       </c>
       <c r="B17" t="n">
-        <v>5065.35567788628</v>
+        <v>5098.35374801361</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.526625500387124</v>
+        <v>0.550097147181697</v>
       </c>
       <c r="D17" t="n">
-        <v>0.150828960461144</v>
+        <v>0.150647984388595</v>
       </c>
       <c r="E17" t="n">
-        <v>-3.49154100629628</v>
+        <v>3.65154004160272</v>
       </c>
       <c r="F17" t="n">
-        <v>0.000480242741371908</v>
+        <v>0.00026067244559421</v>
       </c>
       <c r="G17" t="n">
-        <v>0.0014933368302923</v>
+        <v>0.000994192583196522</v>
       </c>
     </row>
     <row r="18">
@@ -976,22 +982,22 @@
         <v>23</v>
       </c>
       <c r="B18" t="n">
-        <v>10910.0069563415</v>
+        <v>10611.2646574571</v>
       </c>
       <c r="C18" t="n">
-        <v>0.773285873200732</v>
+        <v>-0.752063704267384</v>
       </c>
       <c r="D18" t="n">
-        <v>0.112426155503158</v>
+        <v>0.113410597310908</v>
       </c>
       <c r="E18" t="n">
-        <v>6.87816700428766</v>
+        <v>-6.63133536106553</v>
       </c>
       <c r="F18" t="n">
-        <v>0.00000000000606275722984755</v>
+        <v>0.0000000000332663453576099</v>
       </c>
       <c r="G18" t="n">
-        <v>0.000000000129916226353876</v>
+        <v>0.000000000681960079831002</v>
       </c>
     </row>
     <row r="19">
@@ -999,22 +1005,22 @@
         <v>24</v>
       </c>
       <c r="B19" t="n">
-        <v>4552.32756810648</v>
+        <v>4620.21290989716</v>
       </c>
       <c r="C19" t="n">
-        <v>0.294726606842678</v>
+        <v>-0.252901173532621</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0766821209579116</v>
+        <v>0.0852360378839143</v>
       </c>
       <c r="E19" t="n">
-        <v>3.84348532827417</v>
+        <v>-2.96706862274682</v>
       </c>
       <c r="F19" t="n">
-        <v>0.000121299254213448</v>
+        <v>0.00300653847504591</v>
       </c>
       <c r="G19" t="n">
-        <v>0.000454872203300428</v>
+        <v>0.0088179964228308</v>
       </c>
     </row>
     <row r="20">
@@ -1022,22 +1028,22 @@
         <v>25</v>
       </c>
       <c r="B20" t="n">
-        <v>7421.32478438409</v>
+        <v>7717.77556854491</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.584471629527158</v>
+        <v>0.565753036971677</v>
       </c>
       <c r="D20" t="n">
-        <v>0.106195113104603</v>
+        <v>0.109227725750035</v>
       </c>
       <c r="E20" t="n">
-        <v>-5.50375259689633</v>
+        <v>5.17957352940214</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0000000371791196234561</v>
+        <v>0.000000222393740723054</v>
       </c>
       <c r="G20" t="n">
-        <v>0.00000039343247048877</v>
+        <v>0.00000191960913045163</v>
       </c>
     </row>
     <row r="21">
@@ -1045,22 +1051,22 @@
         <v>26</v>
       </c>
       <c r="B21" t="n">
-        <v>6068.53465385705</v>
+        <v>6039.62499144214</v>
       </c>
       <c r="C21" t="n">
-        <v>0.411061438641751</v>
+        <v>-0.406053383357906</v>
       </c>
       <c r="D21" t="n">
-        <v>0.102172742069492</v>
+        <v>0.102759179074808</v>
       </c>
       <c r="E21" t="n">
-        <v>4.02320061413414</v>
+        <v>-3.95150474160856</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0000574125523294132</v>
+        <v>0.0000776613331982087</v>
       </c>
       <c r="G21" t="n">
-        <v>0.000226628496037158</v>
+        <v>0.000353790517902951</v>
       </c>
     </row>
     <row r="22">
@@ -1068,22 +1074,22 @@
         <v>27</v>
       </c>
       <c r="B22" t="n">
-        <v>5948.64868675816</v>
+        <v>5797.30194393366</v>
       </c>
       <c r="C22" t="n">
-        <v>0.400422180840282</v>
+        <v>-0.428309646243159</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0818666116251795</v>
+        <v>0.0814960820533568</v>
       </c>
       <c r="E22" t="n">
-        <v>4.89115370590378</v>
+        <v>-5.25558573432692</v>
       </c>
       <c r="F22" t="n">
-        <v>0.00000100246640202998</v>
+        <v>0.000000147554094428701</v>
       </c>
       <c r="G22" t="n">
-        <v>0.00000601479841217987</v>
+        <v>0.00000142346302860629</v>
       </c>
     </row>
     <row r="23">
@@ -1091,22 +1097,22 @@
         <v>28</v>
       </c>
       <c r="B23" t="n">
-        <v>6597.94265024403</v>
+        <v>6549.65180921894</v>
       </c>
       <c r="C23" t="n">
-        <v>0.285299037838778</v>
+        <v>-0.357019259564785</v>
       </c>
       <c r="D23" t="n">
-        <v>0.105580696847292</v>
+        <v>0.116185936403236</v>
       </c>
       <c r="E23" t="n">
-        <v>2.70218938080532</v>
+        <v>-3.07282680345848</v>
       </c>
       <c r="F23" t="n">
-        <v>0.00688845145698735</v>
+        <v>0.00212041515177142</v>
       </c>
       <c r="G23" t="n">
-        <v>0.0172211286424684</v>
+        <v>0.00656128462057573</v>
       </c>
     </row>
     <row r="24">
@@ -1114,22 +1120,22 @@
         <v>29</v>
       </c>
       <c r="B24" t="n">
-        <v>7722.32463345544</v>
+        <v>7941.37631805149</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.403271242975128</v>
+        <v>0.381010150274015</v>
       </c>
       <c r="D24" t="n">
-        <v>0.138940912447506</v>
+        <v>0.145295635148794</v>
       </c>
       <c r="E24" t="n">
-        <v>-2.90246577391299</v>
+        <v>2.6223096783591</v>
       </c>
       <c r="F24" t="n">
-        <v>0.00370237613807712</v>
+        <v>0.0087336032459268</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0100973894674831</v>
+        <v>0.0231017892311612</v>
       </c>
     </row>
     <row r="25">
@@ -1137,22 +1143,22 @@
         <v>30</v>
       </c>
       <c r="B25" t="n">
-        <v>7341.44913312977</v>
+        <v>7721.40973607825</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.269043282873627</v>
+        <v>0.345064414771037</v>
       </c>
       <c r="D25" t="n">
-        <v>0.113371570956256</v>
+        <v>0.127202991962298</v>
       </c>
       <c r="E25" t="n">
-        <v>-2.37311065379376</v>
+        <v>2.71270674885785</v>
       </c>
       <c r="F25" t="n">
-        <v>0.0176389786759954</v>
+        <v>0.00667361360195094</v>
       </c>
       <c r="G25" t="n">
-        <v>0.0389095117852839</v>
+        <v>0.0182412105119993</v>
       </c>
     </row>
     <row r="26">
@@ -1160,22 +1166,22 @@
         <v>31</v>
       </c>
       <c r="B26" t="n">
-        <v>4839.47620389338</v>
+        <v>5075.1520808009</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.769456922830354</v>
+        <v>0.821843518249527</v>
       </c>
       <c r="D26" t="n">
-        <v>0.138116715228395</v>
+        <v>0.140404799834776</v>
       </c>
       <c r="E26" t="n">
-        <v>-5.57106300680518</v>
+        <v>5.85338620343924</v>
       </c>
       <c r="F26" t="n">
-        <v>0.0000000253189735789948</v>
+        <v>0.00000000481663862494556</v>
       </c>
       <c r="G26" t="n">
-        <v>0.000000316487169737435</v>
+        <v>0.0000000607637488070055</v>
       </c>
     </row>
     <row r="27">
@@ -1183,22 +1189,22 @@
         <v>32</v>
       </c>
       <c r="B27" t="n">
-        <v>5143.91766462216</v>
+        <v>5061.7414027665</v>
       </c>
       <c r="C27" t="n">
-        <v>0.630605751811114</v>
+        <v>-0.630538551665056</v>
       </c>
       <c r="D27" t="n">
-        <v>0.150825066013613</v>
+        <v>0.162958723732278</v>
       </c>
       <c r="E27" t="n">
-        <v>4.18104078107412</v>
+        <v>-3.86931449402462</v>
       </c>
       <c r="F27" t="n">
-        <v>0.0000290177809195807</v>
+        <v>0.000109141785861881</v>
       </c>
       <c r="G27" t="n">
-        <v>0.000124361918226774</v>
+        <v>0.000447481322033711</v>
       </c>
     </row>
     <row r="28">
@@ -1206,22 +1212,22 @@
         <v>33</v>
       </c>
       <c r="B28" t="n">
-        <v>5804.13338640224</v>
+        <v>5992.98707398336</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.348781777275833</v>
+        <v>0.384632581006195</v>
       </c>
       <c r="D28" t="n">
-        <v>0.105064499981817</v>
+        <v>0.109474805737299</v>
       </c>
       <c r="E28" t="n">
-        <v>-3.31969197337061</v>
+        <v>3.51343469774387</v>
       </c>
       <c r="F28" t="n">
-        <v>0.000901168207186086</v>
+        <v>0.000442353132471686</v>
       </c>
       <c r="G28" t="n">
-        <v>0.00265049472701789</v>
+        <v>0.0015435300792629</v>
       </c>
     </row>
     <row r="29">
@@ -1229,22 +1235,22 @@
         <v>34</v>
       </c>
       <c r="B29" t="n">
-        <v>6824.09156883885</v>
+        <v>6051.04446960441</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.44194489452505</v>
+        <v>0.429142250779093</v>
       </c>
       <c r="D29" t="n">
-        <v>0.122968339265551</v>
+        <v>0.17119718813107</v>
       </c>
       <c r="E29" t="n">
-        <v>-3.59397302724132</v>
+        <v>2.50671319700962</v>
       </c>
       <c r="F29" t="n">
-        <v>0.000325673566416981</v>
+        <v>0.0121859543967516</v>
       </c>
       <c r="G29" t="n">
-        <v>0.00113607058052435</v>
+        <v>0.0307461003241118</v>
       </c>
     </row>
     <row r="30">
@@ -1252,22 +1258,22 @@
         <v>35</v>
       </c>
       <c r="B30" t="n">
-        <v>8028.45649066438</v>
+        <v>6826.0230719088</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.390104296464406</v>
+        <v>0.373423318158994</v>
       </c>
       <c r="D30" t="n">
-        <v>0.0895428327781326</v>
+        <v>0.125875419372011</v>
       </c>
       <c r="E30" t="n">
-        <v>-4.35662223721466</v>
+        <v>2.9666103201244</v>
       </c>
       <c r="F30" t="n">
-        <v>0.0000132084941781179</v>
+        <v>0.00301102316877149</v>
       </c>
       <c r="G30" t="n">
-        <v>0.0000619148164599277</v>
+        <v>0.0088179964228308</v>
       </c>
     </row>
     <row r="31">
@@ -1275,22 +1281,22 @@
         <v>36</v>
       </c>
       <c r="B31" t="n">
-        <v>5094.21505624405</v>
+        <v>8183.66414387651</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.273144606823193</v>
+        <v>0.397625359261421</v>
       </c>
       <c r="D31" t="n">
-        <v>0.115802359046171</v>
+        <v>0.0929244111661489</v>
       </c>
       <c r="E31" t="n">
-        <v>-2.35871366587869</v>
+        <v>4.27901941235298</v>
       </c>
       <c r="F31" t="n">
-        <v>0.0183383994101391</v>
+        <v>0.0000187718492197356</v>
       </c>
       <c r="G31" t="n">
-        <v>0.0398660856742155</v>
+        <v>0.0000993091378076333</v>
       </c>
     </row>
     <row r="32">
@@ -1298,22 +1304,22 @@
         <v>37</v>
       </c>
       <c r="B32" t="n">
-        <v>5494.79595373505</v>
+        <v>5583.69054531017</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.250823468360423</v>
+        <v>0.242644999174626</v>
       </c>
       <c r="D32" t="n">
-        <v>0.069536511361578</v>
+        <v>0.0757208745391503</v>
       </c>
       <c r="E32" t="n">
-        <v>-3.60707581454847</v>
+        <v>3.20446641235199</v>
       </c>
       <c r="F32" t="n">
-        <v>0.000309667201781164</v>
+        <v>0.00135313077275467</v>
       </c>
       <c r="G32" t="n">
-        <v>0.00110595429207558</v>
+        <v>0.00435124405356404</v>
       </c>
     </row>
     <row r="33">
@@ -1321,22 +1327,22 @@
         <v>38</v>
       </c>
       <c r="B33" t="n">
-        <v>7574.89800136381</v>
+        <v>7606.03497694737</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.731230876486238</v>
+        <v>0.740507473066003</v>
       </c>
       <c r="D33" t="n">
-        <v>0.223925839619117</v>
+        <v>0.228256656217206</v>
       </c>
       <c r="E33" t="n">
-        <v>-3.26550467659299</v>
+        <v>3.24418786000854</v>
       </c>
       <c r="F33" t="n">
-        <v>0.00109269201150572</v>
+        <v>0.00117786034754336</v>
       </c>
       <c r="G33" t="n">
-        <v>0.00315199618703575</v>
+        <v>0.00386338193994222</v>
       </c>
     </row>
     <row r="34">
@@ -1344,22 +1350,22 @@
         <v>39</v>
       </c>
       <c r="B34" t="n">
-        <v>6453.66420766663</v>
+        <v>6393.1031419378</v>
       </c>
       <c r="C34" t="n">
-        <v>0.62480144001863</v>
+        <v>-0.662437316998146</v>
       </c>
       <c r="D34" t="n">
-        <v>0.120489577008519</v>
+        <v>0.127189393008432</v>
       </c>
       <c r="E34" t="n">
-        <v>5.18552272761696</v>
+        <v>-5.20827485161621</v>
       </c>
       <c r="F34" t="n">
-        <v>0.000000215409814577896</v>
+        <v>0.000000190604446581698</v>
       </c>
       <c r="G34" t="n">
-        <v>0.00000190067483451085</v>
+        <v>0.00000173661829107769</v>
       </c>
     </row>
     <row r="35">
@@ -1367,22 +1373,22 @@
         <v>40</v>
       </c>
       <c r="B35" t="n">
-        <v>4912.31615810132</v>
+        <v>5005.0761926651</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.905475508603442</v>
+        <v>0.960875169308764</v>
       </c>
       <c r="D35" t="n">
-        <v>0.140662931935132</v>
+        <v>0.144126319105359</v>
       </c>
       <c r="E35" t="n">
-        <v>-6.43720059113376</v>
+        <v>6.66689592347356</v>
       </c>
       <c r="F35" t="n">
-        <v>0.000000000121697061127191</v>
+        <v>0.0000000000261270228891056</v>
       </c>
       <c r="G35" t="n">
-        <v>0.00000000202828435211985</v>
+        <v>0.000000000612118821973331</v>
       </c>
     </row>
     <row r="36">
@@ -1390,22 +1396,22 @@
         <v>41</v>
       </c>
       <c r="B36" t="n">
-        <v>7204.36998457604</v>
+        <v>7508.35003245732</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.462137616483092</v>
+        <v>0.501663585398554</v>
       </c>
       <c r="D36" t="n">
-        <v>0.0900795271328377</v>
+        <v>0.09010502609264</v>
       </c>
       <c r="E36" t="n">
-        <v>-5.13032906801998</v>
+        <v>5.56754275707969</v>
       </c>
       <c r="F36" t="n">
-        <v>0.000000289236101153608</v>
+        <v>0.0000000258356695407021</v>
       </c>
       <c r="G36" t="n">
-        <v>0.00000228344290384427</v>
+        <v>0.000000302646414619653</v>
       </c>
     </row>
     <row r="37">
@@ -1413,22 +1419,22 @@
         <v>42</v>
       </c>
       <c r="B37" t="n">
-        <v>4573.79504966062</v>
+        <v>2548.81189259703</v>
       </c>
       <c r="C37" t="n">
-        <v>0.253970673726462</v>
+        <v>1.02745201299528</v>
       </c>
       <c r="D37" t="n">
-        <v>0.110979146200947</v>
+        <v>0.19968080291798</v>
       </c>
       <c r="E37" t="n">
-        <v>2.28845402420563</v>
+        <v>5.14547216347739</v>
       </c>
       <c r="F37" t="n">
-        <v>0.0221110946065227</v>
+        <v>0.000000266848771109694</v>
       </c>
       <c r="G37" t="n">
-        <v>0.0467135801546254</v>
+        <v>0.00000200153654124363</v>
       </c>
     </row>
     <row r="38">
@@ -1436,22 +1442,22 @@
         <v>43</v>
       </c>
       <c r="B38" t="n">
-        <v>2412.99502133319</v>
+        <v>4364.03558925483</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.933091836129421</v>
+        <v>1.03390489899482</v>
       </c>
       <c r="D38" t="n">
-        <v>0.203255522821712</v>
+        <v>0.157260318517857</v>
       </c>
       <c r="E38" t="n">
-        <v>-4.59073300039131</v>
+        <v>6.57448050938175</v>
       </c>
       <c r="F38" t="n">
-        <v>0.00000441692070285175</v>
+        <v>0.0000000000488233245893935</v>
       </c>
       <c r="G38" t="n">
-        <v>0.0000236620751938487</v>
+        <v>0.000000000800702523266053</v>
       </c>
     </row>
     <row r="39">
@@ -1459,22 +1465,22 @@
         <v>44</v>
       </c>
       <c r="B39" t="n">
-        <v>4038.42859088345</v>
+        <v>5746.64404640247</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.95266992270803</v>
+        <v>-0.551578642156688</v>
       </c>
       <c r="D39" t="n">
-        <v>0.143804666902081</v>
+        <v>0.149529920840875</v>
       </c>
       <c r="E39" t="n">
-        <v>-6.6247496915849</v>
+        <v>-3.68875098077301</v>
       </c>
       <c r="F39" t="n">
-        <v>0.0000000000347837087171388</v>
+        <v>0.000225357652023144</v>
       </c>
       <c r="G39" t="n">
-        <v>0.000000000652194538446353</v>
+        <v>0.000879967974566563</v>
       </c>
     </row>
     <row r="40">
@@ -1482,22 +1488,22 @@
         <v>45</v>
       </c>
       <c r="B40" t="n">
-        <v>5835.58749462129</v>
+        <v>4325.98581686911</v>
       </c>
       <c r="C40" t="n">
-        <v>0.515728332150837</v>
+        <v>0.295713575280729</v>
       </c>
       <c r="D40" t="n">
-        <v>0.146762219671209</v>
+        <v>0.113056132266988</v>
       </c>
       <c r="E40" t="n">
-        <v>3.51404014811319</v>
+        <v>2.61563498901933</v>
       </c>
       <c r="F40" t="n">
-        <v>0.000441346101796527</v>
+        <v>0.00890617091128057</v>
       </c>
       <c r="G40" t="n">
-        <v>0.00140855138871232</v>
+        <v>0.023184317927778</v>
       </c>
     </row>
     <row r="41">
@@ -1505,22 +1511,22 @@
         <v>46</v>
       </c>
       <c r="B41" t="n">
-        <v>4170.21713076279</v>
+        <v>5529.26979807732</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.318111953389496</v>
+        <v>0.309474026936412</v>
       </c>
       <c r="D41" t="n">
-        <v>0.110516878443247</v>
+        <v>0.112841737598512</v>
       </c>
       <c r="E41" t="n">
-        <v>-2.87840154255582</v>
+        <v>2.74254928648398</v>
       </c>
       <c r="F41" t="n">
-        <v>0.00399696024860094</v>
+        <v>0.00609643001855852</v>
       </c>
       <c r="G41" t="n">
-        <v>0.0107061435230382</v>
+        <v>0.0169460088651457</v>
       </c>
     </row>
     <row r="42">
@@ -1528,22 +1534,22 @@
         <v>47</v>
       </c>
       <c r="B42" t="n">
-        <v>5517.36836535035</v>
+        <v>4542.49717963328</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.318106827901662</v>
+        <v>0.479985411116127</v>
       </c>
       <c r="D42" t="n">
-        <v>0.111616942538455</v>
+        <v>0.14696034469561</v>
       </c>
       <c r="E42" t="n">
-        <v>-2.84998693448413</v>
+        <v>3.26608795121086</v>
       </c>
       <c r="F42" t="n">
-        <v>0.00437210250565478</v>
+        <v>0.00109044375704358</v>
       </c>
       <c r="G42" t="n">
-        <v>0.0113071616525555</v>
+        <v>0.00364964849296218</v>
       </c>
     </row>
     <row r="43">
@@ -1551,22 +1557,22 @@
         <v>48</v>
       </c>
       <c r="B43" t="n">
-        <v>4524.55274794091</v>
+        <v>6026.93427764393</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.440246650383581</v>
+        <v>0.850535484514884</v>
       </c>
       <c r="D43" t="n">
-        <v>0.138199250101282</v>
+        <v>0.133178487298131</v>
       </c>
       <c r="E43" t="n">
-        <v>-3.18559362703442</v>
+        <v>6.38643298756569</v>
       </c>
       <c r="F43" t="n">
-        <v>0.00144457352510817</v>
+        <v>0.000000000169799790540007</v>
       </c>
       <c r="G43" t="n">
-        <v>0.0040127042364116</v>
+        <v>0.00000000253156051350556</v>
       </c>
     </row>
     <row r="44">
@@ -1574,22 +1580,22 @@
         <v>49</v>
       </c>
       <c r="B44" t="n">
-        <v>5718.13481671794</v>
+        <v>3663.1952121039</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.739845764512866</v>
+        <v>-0.646877601874446</v>
       </c>
       <c r="D44" t="n">
-        <v>0.134669842100539</v>
+        <v>0.135009564132902</v>
       </c>
       <c r="E44" t="n">
-        <v>-5.49377464897097</v>
+        <v>-4.79134649481326</v>
       </c>
       <c r="F44" t="n">
-        <v>0.000000039343247048877</v>
+        <v>0.00000165665743201273</v>
       </c>
       <c r="G44" t="n">
-        <v>0.00000039343247048877</v>
+        <v>0.000010449685340388</v>
       </c>
     </row>
     <row r="45">
@@ -1597,22 +1603,22 @@
         <v>50</v>
       </c>
       <c r="B45" t="n">
-        <v>3665.2874015089</v>
+        <v>4065.72677753591</v>
       </c>
       <c r="C45" t="n">
-        <v>0.589173736801957</v>
+        <v>-0.919014811569757</v>
       </c>
       <c r="D45" t="n">
-        <v>0.132843849775498</v>
+        <v>0.124044027002178</v>
       </c>
       <c r="E45" t="n">
-        <v>4.43508478411038</v>
+        <v>-7.40877923572746</v>
       </c>
       <c r="F45" t="n">
-        <v>0.0000092036059988047</v>
+        <v>0.000000000000127467288413874</v>
       </c>
       <c r="G45" t="n">
-        <v>0.0000460180299940235</v>
+        <v>0.0000000000069682117666251</v>
       </c>
     </row>
     <row r="46">
@@ -1620,22 +1626,22 @@
         <v>51</v>
       </c>
       <c r="B46" t="n">
-        <v>4160.83036648629</v>
+        <v>4322.03053879335</v>
       </c>
       <c r="C46" t="n">
-        <v>0.98809257669803</v>
+        <v>-0.525130047357311</v>
       </c>
       <c r="D46" t="n">
-        <v>0.124236579662451</v>
+        <v>0.138757915793171</v>
       </c>
       <c r="E46" t="n">
-        <v>7.95331438922951</v>
+        <v>-3.78450515313345</v>
       </c>
       <c r="F46" t="n">
-        <v>0.00000000000000181586754539394</v>
+        <v>0.000154014716612921</v>
       </c>
       <c r="G46" t="n">
-        <v>0.000000000000272380131809091</v>
+        <v>0.000616058866451684</v>
       </c>
     </row>
     <row r="47">
@@ -1643,22 +1649,22 @@
         <v>52</v>
       </c>
       <c r="B47" t="n">
-        <v>4246.01137113803</v>
+        <v>3251.46400141535</v>
       </c>
       <c r="C47" t="n">
-        <v>0.561552995877021</v>
+        <v>0.944147848444847</v>
       </c>
       <c r="D47" t="n">
-        <v>0.136871369594292</v>
+        <v>0.173735284525333</v>
       </c>
       <c r="E47" t="n">
-        <v>4.10277910962351</v>
+        <v>5.43440470958089</v>
       </c>
       <c r="F47" t="n">
-        <v>0.000040821694464912</v>
+        <v>0.0000000549796683136467</v>
       </c>
       <c r="G47" t="n">
-        <v>0.0001700903936038</v>
+        <v>0.000000601111040229204</v>
       </c>
     </row>
     <row r="48">
@@ -1666,22 +1672,22 @@
         <v>53</v>
       </c>
       <c r="B48" t="n">
-        <v>2994.6279516052</v>
+        <v>4505.23195593493</v>
       </c>
       <c r="C48" t="n">
-        <v>-0.819855741049315</v>
+        <v>0.991482921374952</v>
       </c>
       <c r="D48" t="n">
-        <v>0.163966630169142</v>
+        <v>0.18518600508156</v>
       </c>
       <c r="E48" t="n">
-        <v>-5.00013777317728</v>
+        <v>5.35398407097923</v>
       </c>
       <c r="F48" t="n">
-        <v>0.000000572893624685207</v>
+        <v>0.000000086038437666477</v>
       </c>
       <c r="G48" t="n">
-        <v>0.00000409209731918005</v>
+        <v>0.000000881893986081389</v>
       </c>
     </row>
     <row r="49">
@@ -1689,22 +1695,22 @@
         <v>54</v>
       </c>
       <c r="B49" t="n">
-        <v>4251.60378885152</v>
+        <v>3288.73224592805</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.900427315001732</v>
+        <v>0.236630835836353</v>
       </c>
       <c r="D49" t="n">
-        <v>0.183686145411422</v>
+        <v>0.0984210960988094</v>
       </c>
       <c r="E49" t="n">
-        <v>-4.90198818743214</v>
+        <v>2.40426946270532</v>
       </c>
       <c r="F49" t="n">
-        <v>0.000000948715424898129</v>
+        <v>0.0162048235789261</v>
       </c>
       <c r="G49" t="n">
-        <v>0.0000059294714056133</v>
+        <v>0.0385158125644042</v>
       </c>
     </row>
     <row r="50">
@@ -1712,22 +1718,22 @@
         <v>55</v>
       </c>
       <c r="B50" t="n">
-        <v>3261.91806081064</v>
+        <v>2299.32878157692</v>
       </c>
       <c r="C50" t="n">
-        <v>-0.257425322293616</v>
+        <v>0.568496694801543</v>
       </c>
       <c r="D50" t="n">
-        <v>0.0970792871902643</v>
+        <v>0.113691588064585</v>
       </c>
       <c r="E50" t="n">
-        <v>-2.65170181759876</v>
+        <v>5.00034087375572</v>
       </c>
       <c r="F50" t="n">
-        <v>0.00800872346121883</v>
+        <v>0.000000572290439704376</v>
       </c>
       <c r="G50" t="n">
-        <v>0.0190683891933782</v>
+        <v>0.0000039106513379799</v>
       </c>
     </row>
     <row r="51">
@@ -1735,22 +1741,22 @@
         <v>56</v>
       </c>
       <c r="B51" t="n">
-        <v>2232.43699437358</v>
+        <v>2354.03919053216</v>
       </c>
       <c r="C51" t="n">
-        <v>-0.516305269291689</v>
+        <v>0.878685429287322</v>
       </c>
       <c r="D51" t="n">
-        <v>0.117131146215969</v>
+        <v>0.11991457648687</v>
       </c>
       <c r="E51" t="n">
-        <v>-4.40792467222778</v>
+        <v>7.32759481816236</v>
       </c>
       <c r="F51" t="n">
-        <v>0.0000104365827651913</v>
+        <v>0.000000000000234319881455019</v>
       </c>
       <c r="G51" t="n">
-        <v>0.000050499594025119</v>
+        <v>0.00000000000960711513965577</v>
       </c>
     </row>
     <row r="52">
@@ -1758,22 +1764,22 @@
         <v>57</v>
       </c>
       <c r="B52" t="n">
-        <v>2277.38495617882</v>
+        <v>2572.99194919028</v>
       </c>
       <c r="C52" t="n">
-        <v>-0.897745816416929</v>
+        <v>-0.250701150415346</v>
       </c>
       <c r="D52" t="n">
-        <v>0.117439363150393</v>
+        <v>0.0766250760067626</v>
       </c>
       <c r="E52" t="n">
-        <v>-7.64433484935777</v>
+        <v>-3.27178990847878</v>
       </c>
       <c r="F52" t="n">
-        <v>0.0000000000000210028187710401</v>
+        <v>0.00106868958232139</v>
       </c>
       <c r="G52" t="n">
-        <v>0.00000000000147267534690171</v>
+        <v>0.00364964849296218</v>
       </c>
     </row>
     <row r="53">
@@ -1781,22 +1787,22 @@
         <v>58</v>
       </c>
       <c r="B53" t="n">
-        <v>2558.2699326899</v>
+        <v>3369.24745345201</v>
       </c>
       <c r="C53" t="n">
-        <v>0.249532046538177</v>
+        <v>0.45262128792426</v>
       </c>
       <c r="D53" t="n">
-        <v>0.0727378670245663</v>
+        <v>0.114135413687476</v>
       </c>
       <c r="E53" t="n">
-        <v>3.43056590391771</v>
+        <v>3.96565161767951</v>
       </c>
       <c r="F53" t="n">
-        <v>0.000602323639923348</v>
+        <v>0.0000731957068588537</v>
       </c>
       <c r="G53" t="n">
-        <v>0.00180697091977004</v>
+        <v>0.000342974169281486</v>
       </c>
     </row>
     <row r="54">
@@ -1804,22 +1810,22 @@
         <v>59</v>
       </c>
       <c r="B54" t="n">
-        <v>3268.40037114691</v>
+        <v>2955.08576057626</v>
       </c>
       <c r="C54" t="n">
-        <v>-0.45011390455328</v>
+        <v>-0.586199487453224</v>
       </c>
       <c r="D54" t="n">
-        <v>0.106807597505845</v>
+        <v>0.16403039417269</v>
       </c>
       <c r="E54" t="n">
-        <v>-4.21424987607879</v>
+        <v>-3.57372479905205</v>
       </c>
       <c r="F54" t="n">
-        <v>0.0000250609709860119</v>
+        <v>0.000351938822926458</v>
       </c>
       <c r="G54" t="n">
-        <v>0.000113913504481872</v>
+        <v>0.00128262148799864</v>
       </c>
     </row>
     <row r="55">
@@ -1827,22 +1833,22 @@
         <v>60</v>
       </c>
       <c r="B55" t="n">
-        <v>2899.58345081098</v>
+        <v>2907.70522473202</v>
       </c>
       <c r="C55" t="n">
-        <v>0.631837464599288</v>
+        <v>0.557258116596177</v>
       </c>
       <c r="D55" t="n">
-        <v>0.156686550293892</v>
+        <v>0.128716949991592</v>
       </c>
       <c r="E55" t="n">
-        <v>4.0324933021639</v>
+        <v>4.32932971634721</v>
       </c>
       <c r="F55" t="n">
-        <v>0.0000551881884017242</v>
+        <v>0.0000149563866157605</v>
       </c>
       <c r="G55" t="n">
-        <v>0.000223735898925909</v>
+        <v>0.0000817615801661574</v>
       </c>
     </row>
     <row r="56">
@@ -1850,22 +1856,22 @@
         <v>61</v>
       </c>
       <c r="B56" t="n">
-        <v>2836.77752043672</v>
+        <v>1266.8312289158</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.639726369964524</v>
+        <v>-0.618134569713431</v>
       </c>
       <c r="D56" t="n">
-        <v>0.126930324444093</v>
+        <v>0.123083738333825</v>
       </c>
       <c r="E56" t="n">
-        <v>-5.03998057805559</v>
+        <v>-5.02206528726759</v>
       </c>
       <c r="F56" t="n">
-        <v>0.000000465579092273748</v>
+        <v>0.000000511187998335486</v>
       </c>
       <c r="G56" t="n">
-        <v>0.00000349184319205311</v>
+        <v>0.00000364499268378346</v>
       </c>
     </row>
     <row r="57">
@@ -1873,22 +1879,22 @@
         <v>62</v>
       </c>
       <c r="B57" t="n">
-        <v>1242.58435926881</v>
+        <v>2001.67908809915</v>
       </c>
       <c r="C57" t="n">
-        <v>0.640454536533375</v>
+        <v>0.657366410954963</v>
       </c>
       <c r="D57" t="n">
-        <v>0.115876792980199</v>
+        <v>0.167304862484783</v>
       </c>
       <c r="E57" t="n">
-        <v>5.52703021944018</v>
+        <v>3.92915305145272</v>
       </c>
       <c r="F57" t="n">
-        <v>0.0000000325696877845141</v>
+        <v>0.0000852455725148747</v>
       </c>
       <c r="G57" t="n">
-        <v>0.000000375804089821317</v>
+        <v>0.000377280930157106</v>
       </c>
     </row>
     <row r="58">
@@ -1896,22 +1902,22 @@
         <v>63</v>
       </c>
       <c r="B58" t="n">
-        <v>1942.48436562077</v>
+        <v>4420.48039864463</v>
       </c>
       <c r="C58" t="n">
-        <v>-0.549071222061653</v>
+        <v>0.748198494069628</v>
       </c>
       <c r="D58" t="n">
-        <v>0.169977737901432</v>
+        <v>0.144810523150409</v>
       </c>
       <c r="E58" t="n">
-        <v>-3.2302537311095</v>
+        <v>5.16674118560087</v>
       </c>
       <c r="F58" t="n">
-        <v>0.00123680403404026</v>
+        <v>0.000000238210755948349</v>
       </c>
       <c r="G58" t="n">
-        <v>0.00350038877558564</v>
+        <v>0.00000195332819877646</v>
       </c>
     </row>
     <row r="59">
@@ -1919,22 +1925,22 @@
         <v>64</v>
       </c>
       <c r="B59" t="n">
-        <v>4258.07485505037</v>
+        <v>2302.01202972758</v>
       </c>
       <c r="C59" t="n">
-        <v>-0.729736100486113</v>
+        <v>1.11784605865528</v>
       </c>
       <c r="D59" t="n">
-        <v>0.140306666786081</v>
+        <v>0.164773144472494</v>
       </c>
       <c r="E59" t="n">
-        <v>-5.20100802906757</v>
+        <v>6.78415200628692</v>
       </c>
       <c r="F59" t="n">
-        <v>0.000000198210538370089</v>
+        <v>0.0000000000116770333874025</v>
       </c>
       <c r="G59" t="n">
-        <v>0.00000185822379721959</v>
+        <v>0.000000000319172245922336</v>
       </c>
     </row>
     <row r="60">
@@ -1942,22 +1948,22 @@
         <v>65</v>
       </c>
       <c r="B60" t="n">
-        <v>2183.74655527119</v>
+        <v>2984.07156144202</v>
       </c>
       <c r="C60" t="n">
-        <v>-1.15617731798313</v>
+        <v>-0.448329928779044</v>
       </c>
       <c r="D60" t="n">
-        <v>0.160018999746855</v>
+        <v>0.180447927038924</v>
       </c>
       <c r="E60" t="n">
-        <v>-7.22525025035882</v>
+        <v>-2.48453909189179</v>
       </c>
       <c r="F60" t="n">
-        <v>0.000000000000500179902633349</v>
+        <v>0.0129719264816482</v>
       </c>
       <c r="G60" t="n">
-        <v>0.0000000000150053970790005</v>
+        <v>0.0317521782535866</v>
       </c>
     </row>
     <row r="61">
@@ -1965,22 +1971,22 @@
         <v>66</v>
       </c>
       <c r="B61" t="n">
-        <v>2237.0854131929</v>
+        <v>1895.49368950804</v>
       </c>
       <c r="C61" t="n">
-        <v>0.548566400043841</v>
+        <v>1.1353713958136</v>
       </c>
       <c r="D61" t="n">
-        <v>0.24205728938683</v>
+        <v>0.410551639625036</v>
       </c>
       <c r="E61" t="n">
-        <v>2.26626680581877</v>
+        <v>2.76547767986156</v>
       </c>
       <c r="F61" t="n">
-        <v>0.0234350525026083</v>
+        <v>0.00568394947133686</v>
       </c>
       <c r="G61" t="n">
-        <v>0.0488230260471006</v>
+        <v>0.0163031373110529</v>
       </c>
     </row>
     <row r="62">
@@ -1988,22 +1994,22 @@
         <v>67</v>
       </c>
       <c r="B62" t="n">
-        <v>1763.9014050878</v>
+        <v>2199.79265486269</v>
       </c>
       <c r="C62" t="n">
-        <v>0.935889799282176</v>
+        <v>-0.608992015913912</v>
       </c>
       <c r="D62" t="n">
-        <v>0.223377919148885</v>
+        <v>0.261804600903973</v>
       </c>
       <c r="E62" t="n">
-        <v>4.18971491384693</v>
+        <v>-2.32613183195082</v>
       </c>
       <c r="F62" t="n">
-        <v>0.0000279305139313939</v>
+        <v>0.0200115188633056</v>
       </c>
       <c r="G62" t="n">
-        <v>0.000123222855579679</v>
+        <v>0.0455817929664183</v>
       </c>
     </row>
     <row r="63">
@@ -2011,22 +2017,22 @@
         <v>68</v>
       </c>
       <c r="B63" t="n">
-        <v>2259.07753671703</v>
+        <v>1730.92595552647</v>
       </c>
       <c r="C63" t="n">
-        <v>-0.45371219391319</v>
+        <v>-0.977565289032188</v>
       </c>
       <c r="D63" t="n">
-        <v>0.127014237338506</v>
+        <v>0.23312517259669</v>
       </c>
       <c r="E63" t="n">
-        <v>-3.57213650548481</v>
+        <v>-4.19330644624718</v>
       </c>
       <c r="F63" t="n">
-        <v>0.000354080755839719</v>
+        <v>0.0000274917655069443</v>
       </c>
       <c r="G63" t="n">
-        <v>0.00118026918613239</v>
+        <v>0.000137053510746956</v>
       </c>
     </row>
     <row r="64">
@@ -2034,22 +2040,22 @@
         <v>69</v>
       </c>
       <c r="B64" t="n">
-        <v>1660.25201969729</v>
+        <v>2316.40800881715</v>
       </c>
       <c r="C64" t="n">
-        <v>-0.360608332941037</v>
+        <v>0.479028902492129</v>
       </c>
       <c r="D64" t="n">
-        <v>0.135914070652814</v>
+        <v>0.133012353104305</v>
       </c>
       <c r="E64" t="n">
-        <v>-2.65320824554063</v>
+        <v>3.60138657284326</v>
       </c>
       <c r="F64" t="n">
-        <v>0.00797306641073862</v>
+        <v>0.000316524515779514</v>
       </c>
       <c r="G64" t="n">
-        <v>0.0190683891933782</v>
+        <v>0.00117977319517818</v>
       </c>
     </row>
     <row r="65">
@@ -2057,22 +2063,22 @@
         <v>70</v>
       </c>
       <c r="B65" t="n">
-        <v>729.361896713802</v>
+        <v>746.352234833483</v>
       </c>
       <c r="C65" t="n">
-        <v>-1.6541615070545</v>
+        <v>1.49982786202186</v>
       </c>
       <c r="D65" t="n">
-        <v>0.578737231302011</v>
+        <v>0.62905135041478</v>
       </c>
       <c r="E65" t="n">
-        <v>-2.85822549092454</v>
+        <v>2.38426936216401</v>
       </c>
       <c r="F65" t="n">
-        <v>0.0042601753640762</v>
+        <v>0.0171130712351183</v>
       </c>
       <c r="G65" t="n">
-        <v>0.0112109878002005</v>
+        <v>0.0399923968274901</v>
       </c>
     </row>
     <row r="66">
@@ -2080,22 +2086,22 @@
         <v>71</v>
       </c>
       <c r="B66" t="n">
-        <v>152.083835352422</v>
+        <v>171.91835390834</v>
       </c>
       <c r="C66" t="n">
-        <v>-5.57217475112266</v>
+        <v>6.13237297831303</v>
       </c>
       <c r="D66" t="n">
-        <v>0.776891472305831</v>
+        <v>0.753809126261784</v>
       </c>
       <c r="E66" t="n">
-        <v>-7.17239788278835</v>
+        <v>8.13518006703381</v>
       </c>
       <c r="F66" t="n">
-        <v>0.00000000000073695383446403</v>
+        <v>0.000000000000000411326510000717</v>
       </c>
       <c r="G66" t="n">
-        <v>0.0000000000184238458616008</v>
+        <v>0.0000000000000674575476401177</v>
       </c>
     </row>
     <row r="67">
@@ -2103,22 +2109,22 @@
         <v>72</v>
       </c>
       <c r="B67" t="n">
-        <v>745.592804210546</v>
+        <v>753.194174246436</v>
       </c>
       <c r="C67" t="n">
-        <v>-0.457189357951124</v>
+        <v>0.467207900195248</v>
       </c>
       <c r="D67" t="n">
-        <v>0.162241082089464</v>
+        <v>0.169228291670067</v>
       </c>
       <c r="E67" t="n">
-        <v>-2.81796294787418</v>
+        <v>2.76081437438446</v>
       </c>
       <c r="F67" t="n">
-        <v>0.00483293866110807</v>
+        <v>0.00576574368317726</v>
       </c>
       <c r="G67" t="n">
-        <v>0.0122871321892578</v>
+        <v>0.0163031373110529</v>
       </c>
     </row>
     <row r="68">
@@ -2126,22 +2132,22 @@
         <v>73</v>
       </c>
       <c r="B68" t="n">
-        <v>696.71540719165</v>
+        <v>740.703892787133</v>
       </c>
       <c r="C68" t="n">
-        <v>-0.999477403880616</v>
+        <v>0.930975867561385</v>
       </c>
       <c r="D68" t="n">
-        <v>0.403969080612554</v>
+        <v>0.405398682142628</v>
       </c>
       <c r="E68" t="n">
-        <v>-2.47414332395209</v>
+        <v>2.296445224343</v>
       </c>
       <c r="F68" t="n">
-        <v>0.0133556105538937</v>
+        <v>0.0216504376843712</v>
       </c>
       <c r="G68" t="n">
-        <v>0.0303536603497584</v>
+        <v>0.0479820510842821</v>
       </c>
     </row>
     <row r="69">
@@ -2149,22 +2155,22 @@
         <v>74</v>
       </c>
       <c r="B69" t="n">
-        <v>1049.52654162162</v>
+        <v>1083.0361311981</v>
       </c>
       <c r="C69" t="n">
-        <v>-1.21236444438211</v>
+        <v>1.26235533789556</v>
       </c>
       <c r="D69" t="n">
-        <v>0.206065136324665</v>
+        <v>0.204022651054345</v>
       </c>
       <c r="E69" t="n">
-        <v>-5.88340398577648</v>
+        <v>6.18732935471613</v>
       </c>
       <c r="F69" t="n">
-        <v>0.00000000401913292368842</v>
+        <v>0.000000000611920301929408</v>
       </c>
       <c r="G69" t="n">
-        <v>0.0000000602869938553263</v>
+        <v>0.00000000836291079303524</v>
       </c>
     </row>
     <row r="70">
@@ -2172,22 +2178,22 @@
         <v>75</v>
       </c>
       <c r="B70" t="n">
-        <v>1054.42349218569</v>
+        <v>1087.51098832489</v>
       </c>
       <c r="C70" t="n">
-        <v>-0.411901878211791</v>
+        <v>0.41652130462533</v>
       </c>
       <c r="D70" t="n">
-        <v>0.171464368582961</v>
+        <v>0.17501074122636</v>
       </c>
       <c r="E70" t="n">
-        <v>-2.40225932428928</v>
+        <v>2.37997566153153</v>
       </c>
       <c r="F70" t="n">
-        <v>0.0162941527806353</v>
+        <v>0.0173137815533646</v>
       </c>
       <c r="G70" t="n">
-        <v>0.0364794465238103</v>
+        <v>0.0399923968274901</v>
       </c>
     </row>
     <row r="71">
@@ -2195,22 +2201,22 @@
         <v>76</v>
       </c>
       <c r="B71" t="n">
-        <v>903.384548178115</v>
+        <v>925.133347163617</v>
       </c>
       <c r="C71" t="n">
-        <v>-0.753772768151163</v>
+        <v>0.734411694068904</v>
       </c>
       <c r="D71" t="n">
-        <v>0.152250697773077</v>
+        <v>0.149343849563675</v>
       </c>
       <c r="E71" t="n">
-        <v>-4.95086577057682</v>
+        <v>4.91758914889747</v>
       </c>
       <c r="F71" t="n">
-        <v>0.000000738840522406699</v>
+        <v>0.000000876165591922717</v>
       </c>
       <c r="G71" t="n">
-        <v>0.00000503754901640931</v>
+        <v>0.00000574764628301303</v>
       </c>
     </row>
     <row r="72">
@@ -2218,22 +2224,22 @@
         <v>77</v>
       </c>
       <c r="B72" t="n">
-        <v>1079.68552947688</v>
+        <v>3.7373017954898</v>
       </c>
       <c r="C72" t="n">
-        <v>-0.413772419244859</v>
+        <v>2.14271601345821</v>
       </c>
       <c r="D72" t="n">
-        <v>0.11550480473176</v>
+        <v>0.886992618058577</v>
       </c>
       <c r="E72" t="n">
-        <v>-3.58229616686314</v>
+        <v>2.41570895837682</v>
       </c>
       <c r="F72" t="n">
-        <v>0.000340587345889882</v>
+        <v>0.0157046085593352</v>
       </c>
       <c r="G72" t="n">
-        <v>0.00116109322462459</v>
+        <v>0.0378758206431026</v>
       </c>
     </row>
     <row r="73">
@@ -2241,22 +2247,68 @@
         <v>78</v>
       </c>
       <c r="B73" t="n">
-        <v>332.527634929455</v>
+        <v>1125.30905437804</v>
       </c>
       <c r="C73" t="n">
-        <v>-1.56780721710272</v>
+        <v>0.505280044292394</v>
       </c>
       <c r="D73" t="n">
-        <v>0.324281320870648</v>
+        <v>0.125761750054963</v>
       </c>
       <c r="E73" t="n">
-        <v>-4.83471330662336</v>
+        <v>4.01775614661506</v>
       </c>
       <c r="F73" t="n">
-        <v>0.00000133337660678175</v>
+        <v>0.0000587549528048842</v>
       </c>
       <c r="G73" t="n">
-        <v>0.00000743009008785153</v>
+        <v>0.000283406242941206</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74" t="n">
+        <v>315.782722205069</v>
+      </c>
+      <c r="C74" t="n">
+        <v>1.48942948070024</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.338323659578925</v>
+      </c>
+      <c r="E74" t="n">
+        <v>4.40238049728468</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.0000107069567006646</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0.0000605496861692759</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75" t="n">
+        <v>229.238434405197</v>
+      </c>
+      <c r="C75" t="n">
+        <v>1.18706025375447</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.516537241748522</v>
+      </c>
+      <c r="E75" t="n">
+        <v>2.29811165161329</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.0215554352718635</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0.0479820510842821</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added functional sites from Fig 4
</commit_message>
<xml_diff>
--- a/tables/output/TableS3-DeSeq2-sbi-SFs.xlsx
+++ b/tables/output/TableS3-DeSeq2-sbi-SFs.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t xml:space="preserve">gene</t>
   </si>
@@ -35,6 +35,9 @@
     <t xml:space="preserve">padj</t>
   </si>
   <si>
+    <t xml:space="preserve">HNRNPA1</t>
+  </si>
+  <si>
     <t xml:space="preserve">PABPC1</t>
   </si>
   <si>
@@ -62,9 +65,6 @@
     <t xml:space="preserve">HNRNPUL1</t>
   </si>
   <si>
-    <t xml:space="preserve">SF1</t>
-  </si>
-  <si>
     <t xml:space="preserve">RBM39</t>
   </si>
   <si>
@@ -86,9 +86,6 @@
     <t xml:space="preserve">KHSRP</t>
   </si>
   <si>
-    <t xml:space="preserve">SRSF2</t>
-  </si>
-  <si>
     <t xml:space="preserve">SRSF1</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t xml:space="preserve">HNRNPA0</t>
   </si>
   <si>
-    <t xml:space="preserve">SYNCRIP</t>
-  </si>
-  <si>
     <t xml:space="preserve">HNRNPR</t>
   </si>
   <si>
@@ -119,12 +113,12 @@
     <t xml:space="preserve">RBFOX2</t>
   </si>
   <si>
-    <t xml:space="preserve">G3BP1</t>
-  </si>
-  <si>
     <t xml:space="preserve">CELF1</t>
   </si>
   <si>
+    <t xml:space="preserve">SRRM1</t>
+  </si>
+  <si>
     <t xml:space="preserve">TARDBP</t>
   </si>
   <si>
@@ -149,9 +143,6 @@
     <t xml:space="preserve">U2AF2</t>
   </si>
   <si>
-    <t xml:space="preserve">FXR1</t>
-  </si>
-  <si>
     <t xml:space="preserve">ANKHD1</t>
   </si>
   <si>
@@ -167,18 +158,21 @@
     <t xml:space="preserve">RALY</t>
   </si>
   <si>
+    <t xml:space="preserve">SRSF4</t>
+  </si>
+  <si>
     <t xml:space="preserve">RBM15B</t>
   </si>
   <si>
+    <t xml:space="preserve">HNRNPH2</t>
+  </si>
+  <si>
     <t xml:space="preserve">TIA1</t>
   </si>
   <si>
     <t xml:space="preserve">RBM6</t>
   </si>
   <si>
-    <t xml:space="preserve">TIAL1</t>
-  </si>
-  <si>
     <t xml:space="preserve">TRA2A</t>
   </si>
   <si>
@@ -194,9 +188,18 @@
     <t xml:space="preserve">RBM10</t>
   </si>
   <si>
+    <t xml:space="preserve">DAZAP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RBM22</t>
+  </si>
+  <si>
     <t xml:space="preserve">FMR1</t>
   </si>
   <si>
+    <t xml:space="preserve">SRPK1</t>
+  </si>
+  <si>
     <t xml:space="preserve">SNRPA</t>
   </si>
   <si>
@@ -209,18 +212,21 @@
     <t xml:space="preserve">PTBP2</t>
   </si>
   <si>
-    <t xml:space="preserve">MSI1</t>
+    <t xml:space="preserve">SRSF8</t>
   </si>
   <si>
     <t xml:space="preserve">ELAVL4</t>
   </si>
   <si>
-    <t xml:space="preserve">KHDRBS3</t>
-  </si>
-  <si>
     <t xml:space="preserve">RBM42</t>
   </si>
   <si>
+    <t xml:space="preserve">CLK2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEMIN5</t>
+  </si>
+  <si>
     <t xml:space="preserve">RBM15</t>
   </si>
   <si>
@@ -230,31 +236,52 @@
     <t xml:space="preserve">IGF2BP1</t>
   </si>
   <si>
-    <t xml:space="preserve">RBM7</t>
-  </si>
-  <si>
     <t xml:space="preserve">ELAVL2</t>
   </si>
   <si>
     <t xml:space="preserve">CLK4</t>
   </si>
   <si>
+    <t xml:space="preserve">CELF4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RBFOX1</t>
+  </si>
+  <si>
     <t xml:space="preserve">PRPF40B</t>
   </si>
   <si>
     <t xml:space="preserve">RBM41</t>
   </si>
   <si>
+    <t xml:space="preserve">CPEB3</t>
+  </si>
+  <si>
     <t xml:space="preserve">WT1</t>
   </si>
   <si>
     <t xml:space="preserve">ZC3H10</t>
   </si>
   <si>
+    <t xml:space="preserve">RBFOX3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2AF1L4</t>
+  </si>
+  <si>
     <t xml:space="preserve">CELF6</t>
   </si>
   <si>
+    <t xml:space="preserve">RBM45</t>
+  </si>
+  <si>
     <t xml:space="preserve">RBM24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRPK3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESRP2</t>
   </si>
 </sst>
 </file>
@@ -614,22 +641,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>21413.9444882445</v>
+        <v>26101.3687736019</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.395491771446074</v>
+        <v>-0.320644871996867</v>
       </c>
       <c r="D2" t="n">
-        <v>0.111356706801239</v>
+        <v>0.0943999599831952</v>
       </c>
       <c r="E2" t="n">
-        <v>-3.55157567789778</v>
+        <v>-3.39666321949656</v>
       </c>
       <c r="F2" t="n">
-        <v>0.000382931853913751</v>
+        <v>0.000682128629495445</v>
       </c>
       <c r="G2" t="n">
-        <v>0.00136523530525772</v>
+        <v>0.00216444661282208</v>
       </c>
     </row>
     <row r="3">
@@ -637,22 +664,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>29625.9238314483</v>
+        <v>20406.5799129285</v>
       </c>
       <c r="C3" t="n">
-        <v>0.280456707214421</v>
+        <v>-0.44317046328538</v>
       </c>
       <c r="D3" t="n">
-        <v>0.10989920391986</v>
+        <v>0.107789715153888</v>
       </c>
       <c r="E3" t="n">
-        <v>2.55194484774371</v>
+        <v>-4.11143551731888</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0107123474561109</v>
+        <v>0.0000393206697041356</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0274503903562841</v>
+        <v>0.000175348932464388</v>
       </c>
     </row>
     <row r="4">
@@ -660,22 +687,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>17105.9396699372</v>
+        <v>29509.0486458093</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.359916309398203</v>
+        <v>0.253861013204767</v>
       </c>
       <c r="D4" t="n">
-        <v>0.117419582518479</v>
+        <v>0.0911934597768839</v>
       </c>
       <c r="E4" t="n">
-        <v>-3.06521537275574</v>
+        <v>2.7837633732273</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00217513301296727</v>
+        <v>0.0053732218589672</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00660595952086357</v>
+        <v>0.013639717026609</v>
       </c>
     </row>
     <row r="5">
@@ -683,22 +710,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>17145.0455603426</v>
+        <v>16345.9036910911</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.05740427150994</v>
+        <v>-0.307481487538994</v>
       </c>
       <c r="D5" t="n">
-        <v>0.151913112208005</v>
+        <v>0.116154256875696</v>
       </c>
       <c r="E5" t="n">
-        <v>-6.96058593060819</v>
+        <v>-2.64718225409552</v>
       </c>
       <c r="F5" t="n">
-        <v>0.00000000000338860392151664</v>
+        <v>0.00811655960825656</v>
       </c>
       <c r="G5" t="n">
-        <v>0.000000000111146208625746</v>
+        <v>0.0194091642806135</v>
       </c>
     </row>
     <row r="6">
@@ -706,22 +733,22 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>17025.9790703674</v>
+        <v>15962.0375344305</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.400565512875317</v>
+        <v>-1.0461554216428</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0955411307769207</v>
+        <v>0.17161638799629</v>
       </c>
       <c r="E6" t="n">
-        <v>-4.19259757151712</v>
+        <v>-6.09589465118805</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0000275778405771315</v>
+        <v>0.0000000010882706916547</v>
       </c>
       <c r="G6" t="n">
-        <v>0.000137053510746956</v>
+        <v>0.0000000138126664710019</v>
       </c>
     </row>
     <row r="7">
@@ -729,22 +756,22 @@
         <v>12</v>
       </c>
       <c r="B7" t="n">
-        <v>15331.6791294024</v>
+        <v>17505.6204180942</v>
       </c>
       <c r="C7" t="n">
-        <v>0.288425447691839</v>
+        <v>-0.420512533871336</v>
       </c>
       <c r="D7" t="n">
-        <v>0.11601132410771</v>
+        <v>0.076045050857833</v>
       </c>
       <c r="E7" t="n">
-        <v>2.48618356794249</v>
+        <v>-5.52978174289723</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0129121342430727</v>
+        <v>0.0000000320629456790397</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0317521782535866</v>
+        <v>0.000000311199178649503</v>
       </c>
     </row>
     <row r="8">
@@ -752,22 +779,22 @@
         <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>10965.1673681756</v>
+        <v>14915.0307671193</v>
       </c>
       <c r="C8" t="n">
-        <v>0.323770095545052</v>
+        <v>0.319300362366395</v>
       </c>
       <c r="D8" t="n">
-        <v>0.121795156030433</v>
+        <v>0.10636663964766</v>
       </c>
       <c r="E8" t="n">
-        <v>2.65831668596207</v>
+        <v>3.00188445760887</v>
       </c>
       <c r="F8" t="n">
-        <v>0.00785320603531949</v>
+        <v>0.00268313993821384</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0211135375375803</v>
+        <v>0.00776698403167165</v>
       </c>
     </row>
     <row r="9">
@@ -775,22 +802,22 @@
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>12811.145790085</v>
+        <v>10929.9070006073</v>
       </c>
       <c r="C9" t="n">
-        <v>0.368747547359242</v>
+        <v>0.32617556054346</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0939940457858326</v>
+        <v>0.0988350871706488</v>
       </c>
       <c r="E9" t="n">
-        <v>3.9230947479316</v>
+        <v>3.30020005931987</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0000874187521095733</v>
+        <v>0.000966159280295343</v>
       </c>
       <c r="G9" t="n">
-        <v>0.000377280930157106</v>
+        <v>0.00300785436318361</v>
       </c>
     </row>
     <row r="10">
@@ -798,22 +825,22 @@
         <v>15</v>
       </c>
       <c r="B10" t="n">
-        <v>12081.3644648276</v>
+        <v>13055.1164126614</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.68018014357471</v>
+        <v>0.217501549450451</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0912297827168843</v>
+        <v>0.0810060693694142</v>
       </c>
       <c r="E10" t="n">
-        <v>-7.45568084586511</v>
+        <v>2.68500312561239</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0000000000000894049280531944</v>
+        <v>0.00725291279225187</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0000000000069682117666251</v>
+        <v>0.0175989795694347</v>
       </c>
     </row>
     <row r="11">
@@ -821,22 +848,22 @@
         <v>16</v>
       </c>
       <c r="B11" t="n">
-        <v>9649.38986704767</v>
+        <v>11260.7603226445</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.331899210302079</v>
+        <v>-0.560469990592832</v>
       </c>
       <c r="D11" t="n">
-        <v>0.105689379681092</v>
+        <v>0.119736766553321</v>
       </c>
       <c r="E11" t="n">
-        <v>-3.14032697801381</v>
+        <v>-4.68085122662173</v>
       </c>
       <c r="F11" t="n">
-        <v>0.00168759360998896</v>
+        <v>0.00000285686210198414</v>
       </c>
       <c r="G11" t="n">
-        <v>0.00532241061611903</v>
+        <v>0.0000168350802438351</v>
       </c>
     </row>
     <row r="12">
@@ -844,22 +871,22 @@
         <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>8275.86662467782</v>
+        <v>8552.93893300786</v>
       </c>
       <c r="C12" t="n">
-        <v>0.810126221942985</v>
+        <v>0.738463907975456</v>
       </c>
       <c r="D12" t="n">
-        <v>0.122569147726487</v>
+        <v>0.10187530835006</v>
       </c>
       <c r="E12" t="n">
-        <v>6.60954438347555</v>
+        <v>7.24870353705308</v>
       </c>
       <c r="F12" t="n">
-        <v>0.000000000038550463205887</v>
+        <v>0.000000000000420779752875348</v>
       </c>
       <c r="G12" t="n">
-        <v>0.000000000702475107307274</v>
+        <v>0.0000000000138857318448865</v>
       </c>
     </row>
     <row r="13">
@@ -867,22 +894,22 @@
         <v>18</v>
       </c>
       <c r="B13" t="n">
-        <v>7060.39441006975</v>
+        <v>6545.29220362266</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.670978616162992</v>
+        <v>-0.617603512193518</v>
       </c>
       <c r="D13" t="n">
-        <v>0.173076512901772</v>
+        <v>0.169756776215262</v>
       </c>
       <c r="E13" t="n">
-        <v>-3.87677452540196</v>
+        <v>-3.63816706444967</v>
       </c>
       <c r="F13" t="n">
-        <v>0.000105850365725583</v>
+        <v>0.000274585294493193</v>
       </c>
       <c r="G13" t="n">
-        <v>0.000445114358435784</v>
+        <v>0.000963969650880358</v>
       </c>
     </row>
     <row r="14">
@@ -890,22 +917,22 @@
         <v>19</v>
       </c>
       <c r="B14" t="n">
-        <v>8003.06222793178</v>
+        <v>7788.35265748879</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.367145514669166</v>
+        <v>-0.269208862320926</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0778183001408533</v>
+        <v>0.0785002198798365</v>
       </c>
       <c r="E14" t="n">
-        <v>-4.71798425312069</v>
+        <v>-3.42940265305008</v>
       </c>
       <c r="F14" t="n">
-        <v>0.00000238192925672816</v>
+        <v>0.00060491138537739</v>
       </c>
       <c r="G14" t="n">
-        <v>0.000014468014744571</v>
+        <v>0.00201023687707711</v>
       </c>
     </row>
     <row r="15">
@@ -913,22 +940,22 @@
         <v>20</v>
       </c>
       <c r="B15" t="n">
-        <v>6144.14236279482</v>
+        <v>6037.8662283942</v>
       </c>
       <c r="C15" t="n">
-        <v>0.747952249287623</v>
+        <v>0.680262606662735</v>
       </c>
       <c r="D15" t="n">
-        <v>0.145393946657754</v>
+        <v>0.118735759279534</v>
       </c>
       <c r="E15" t="n">
-        <v>5.14431492150251</v>
+        <v>5.72921427201407</v>
       </c>
       <c r="F15" t="n">
-        <v>0.00000026849880431317</v>
+        <v>0.0000000100896882091834</v>
       </c>
       <c r="G15" t="n">
-        <v>0.00000200153654124363</v>
+        <v>0.000000104049909657204</v>
       </c>
     </row>
     <row r="16">
@@ -936,22 +963,22 @@
         <v>21</v>
       </c>
       <c r="B16" t="n">
-        <v>6995.87319487614</v>
+        <v>6392.2732441883</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.716777030358966</v>
+        <v>-0.656231233593794</v>
       </c>
       <c r="D16" t="n">
-        <v>0.154317974837913</v>
+        <v>0.168956386558474</v>
       </c>
       <c r="E16" t="n">
-        <v>-4.64480583750419</v>
+        <v>-3.88402739287205</v>
       </c>
       <c r="F16" t="n">
-        <v>0.00000340396437982646</v>
+        <v>0.000102740324942023</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0000199375056532693</v>
+        <v>0.00044610930566931</v>
       </c>
     </row>
     <row r="17">
@@ -959,22 +986,22 @@
         <v>22</v>
       </c>
       <c r="B17" t="n">
-        <v>5098.35374801361</v>
+        <v>5658.72900733722</v>
       </c>
       <c r="C17" t="n">
-        <v>0.550097147181697</v>
+        <v>0.553461333406723</v>
       </c>
       <c r="D17" t="n">
-        <v>0.150647984388595</v>
+        <v>0.127128150096726</v>
       </c>
       <c r="E17" t="n">
-        <v>3.65154004160272</v>
+        <v>4.35357025950288</v>
       </c>
       <c r="F17" t="n">
-        <v>0.00026067244559421</v>
+        <v>0.0000133938142267016</v>
       </c>
       <c r="G17" t="n">
-        <v>0.000994192583196522</v>
+        <v>0.0000649993925707576</v>
       </c>
     </row>
     <row r="18">
@@ -982,22 +1009,22 @@
         <v>23</v>
       </c>
       <c r="B18" t="n">
-        <v>10611.2646574571</v>
+        <v>10159.0121177212</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.752063704267384</v>
+        <v>-0.653207747066494</v>
       </c>
       <c r="D18" t="n">
-        <v>0.113410597310908</v>
+        <v>0.127420021227214</v>
       </c>
       <c r="E18" t="n">
-        <v>-6.63133536106553</v>
+        <v>-5.12641373604626</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0000000000332663453576099</v>
+        <v>0.000000295313269579978</v>
       </c>
       <c r="G18" t="n">
-        <v>0.000000000681960079831002</v>
+        <v>0.00000211855171655202</v>
       </c>
     </row>
     <row r="19">
@@ -1005,22 +1032,22 @@
         <v>24</v>
       </c>
       <c r="B19" t="n">
-        <v>4620.21290989716</v>
+        <v>7828.91681356331</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.252901173532621</v>
+        <v>0.425228745844801</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0852360378839143</v>
+        <v>0.0938355233717226</v>
       </c>
       <c r="E19" t="n">
-        <v>-2.96706862274682</v>
+        <v>4.53163930423544</v>
       </c>
       <c r="F19" t="n">
-        <v>0.00300653847504591</v>
+        <v>0.00000585277219238843</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0088179964228308</v>
+        <v>0.0000301783566170028</v>
       </c>
     </row>
     <row r="20">
@@ -1028,22 +1055,22 @@
         <v>25</v>
       </c>
       <c r="B20" t="n">
-        <v>7717.77556854491</v>
+        <v>5838.82063149871</v>
       </c>
       <c r="C20" t="n">
-        <v>0.565753036971677</v>
+        <v>-0.34146023304903</v>
       </c>
       <c r="D20" t="n">
-        <v>0.109227725750035</v>
+        <v>0.0997802843273654</v>
       </c>
       <c r="E20" t="n">
-        <v>5.17957352940214</v>
+        <v>-3.42212126725101</v>
       </c>
       <c r="F20" t="n">
-        <v>0.000000222393740723054</v>
+        <v>0.000621345943823836</v>
       </c>
       <c r="G20" t="n">
-        <v>0.00000191960913045163</v>
+        <v>0.00201023687707711</v>
       </c>
     </row>
     <row r="21">
@@ -1051,22 +1078,22 @@
         <v>26</v>
       </c>
       <c r="B21" t="n">
-        <v>6039.62499144214</v>
+        <v>5858.76044760758</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.406053383357906</v>
+        <v>-0.377563712654433</v>
       </c>
       <c r="D21" t="n">
-        <v>0.102759179074808</v>
+        <v>0.0724911021698273</v>
       </c>
       <c r="E21" t="n">
-        <v>-3.95150474160856</v>
+        <v>-5.20841456886532</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0000776613331982087</v>
+        <v>0.000000190461007181549</v>
       </c>
       <c r="G21" t="n">
-        <v>0.000353790517902951</v>
+        <v>0.00000157130330924778</v>
       </c>
     </row>
     <row r="22">
@@ -1074,22 +1101,22 @@
         <v>27</v>
       </c>
       <c r="B22" t="n">
-        <v>5797.30194393366</v>
+        <v>6492.75220268824</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.428309646243159</v>
+        <v>-0.336171020685455</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0814960820533568</v>
+        <v>0.094032062649308</v>
       </c>
       <c r="E22" t="n">
-        <v>-5.25558573432692</v>
+        <v>-3.57506802694739</v>
       </c>
       <c r="F22" t="n">
-        <v>0.000000147554094428701</v>
+        <v>0.000350136843850771</v>
       </c>
       <c r="G22" t="n">
-        <v>0.00000142346302860629</v>
+        <v>0.00120359540073702</v>
       </c>
     </row>
     <row r="23">
@@ -1097,22 +1124,22 @@
         <v>28</v>
       </c>
       <c r="B23" t="n">
-        <v>6549.65180921894</v>
+        <v>7582.75983597927</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.357019259564785</v>
+        <v>0.280405437776756</v>
       </c>
       <c r="D23" t="n">
-        <v>0.116185936403236</v>
+        <v>0.107609136674634</v>
       </c>
       <c r="E23" t="n">
-        <v>-3.07282680345848</v>
+        <v>2.60577722711955</v>
       </c>
       <c r="F23" t="n">
-        <v>0.00212041515177142</v>
+        <v>0.0091666059445717</v>
       </c>
       <c r="G23" t="n">
-        <v>0.00656128462057573</v>
+        <v>0.0204390537953288</v>
       </c>
     </row>
     <row r="24">
@@ -1120,22 +1147,22 @@
         <v>29</v>
       </c>
       <c r="B24" t="n">
-        <v>7941.37631805149</v>
+        <v>5053.08820766381</v>
       </c>
       <c r="C24" t="n">
-        <v>0.381010150274015</v>
+        <v>0.848808958853837</v>
       </c>
       <c r="D24" t="n">
-        <v>0.145295635148794</v>
+        <v>0.116343699251245</v>
       </c>
       <c r="E24" t="n">
-        <v>2.6223096783591</v>
+        <v>7.2957019960387</v>
       </c>
       <c r="F24" t="n">
-        <v>0.0087336032459268</v>
+        <v>0.000000000000297105858505992</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0231017892311612</v>
+        <v>0.0000000000122556166633722</v>
       </c>
     </row>
     <row r="25">
@@ -1143,22 +1170,22 @@
         <v>30</v>
       </c>
       <c r="B25" t="n">
-        <v>7721.40973607825</v>
+        <v>4968.98096905882</v>
       </c>
       <c r="C25" t="n">
-        <v>0.345064414771037</v>
+        <v>-0.704201131123144</v>
       </c>
       <c r="D25" t="n">
-        <v>0.127202991962298</v>
+        <v>0.131812820797718</v>
       </c>
       <c r="E25" t="n">
-        <v>2.71270674885785</v>
+        <v>-5.34243275321313</v>
       </c>
       <c r="F25" t="n">
-        <v>0.00667361360195094</v>
+        <v>0.0000000917073970980957</v>
       </c>
       <c r="G25" t="n">
-        <v>0.0182412105119993</v>
+        <v>0.000000796406343220304</v>
       </c>
     </row>
     <row r="26">
@@ -1166,22 +1193,22 @@
         <v>31</v>
       </c>
       <c r="B26" t="n">
-        <v>5075.1520808009</v>
+        <v>6037.40182141618</v>
       </c>
       <c r="C26" t="n">
-        <v>0.821843518249527</v>
+        <v>0.245915742698798</v>
       </c>
       <c r="D26" t="n">
-        <v>0.140404799834776</v>
+        <v>0.0937105128081939</v>
       </c>
       <c r="E26" t="n">
-        <v>5.85338620343924</v>
+        <v>2.62420656263121</v>
       </c>
       <c r="F26" t="n">
-        <v>0.00000000481663862494556</v>
+        <v>0.00868510944818803</v>
       </c>
       <c r="G26" t="n">
-        <v>0.0000000607637488070055</v>
+        <v>0.0197813052325579</v>
       </c>
     </row>
     <row r="27">
@@ -1189,22 +1216,22 @@
         <v>32</v>
       </c>
       <c r="B27" t="n">
-        <v>5061.7414027665</v>
+        <v>6754.69586959233</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.630538551665056</v>
+        <v>0.564117607978774</v>
       </c>
       <c r="D27" t="n">
-        <v>0.162958723732278</v>
+        <v>0.149189901514856</v>
       </c>
       <c r="E27" t="n">
-        <v>-3.86931449402462</v>
+        <v>3.78120504304106</v>
       </c>
       <c r="F27" t="n">
-        <v>0.000109141785861881</v>
+        <v>0.000156071060201751</v>
       </c>
       <c r="G27" t="n">
-        <v>0.000447481322033711</v>
+        <v>0.000613136307935451</v>
       </c>
     </row>
     <row r="28">
@@ -1212,22 +1239,22 @@
         <v>33</v>
       </c>
       <c r="B28" t="n">
-        <v>5992.98707398336</v>
+        <v>8343.65883532118</v>
       </c>
       <c r="C28" t="n">
-        <v>0.384632581006195</v>
+        <v>0.429748378937869</v>
       </c>
       <c r="D28" t="n">
-        <v>0.109474805737299</v>
+        <v>0.0744855863391361</v>
       </c>
       <c r="E28" t="n">
-        <v>3.51343469774387</v>
+        <v>5.76955086291737</v>
       </c>
       <c r="F28" t="n">
-        <v>0.000442353132471686</v>
+        <v>0.00000000794830861443028</v>
       </c>
       <c r="G28" t="n">
-        <v>0.0015435300792629</v>
+        <v>0.0000000874313947587331</v>
       </c>
     </row>
     <row r="29">
@@ -1235,22 +1262,22 @@
         <v>34</v>
       </c>
       <c r="B29" t="n">
-        <v>6051.04446960441</v>
+        <v>4839.73557895629</v>
       </c>
       <c r="C29" t="n">
-        <v>0.429142250779093</v>
+        <v>0.357828685579695</v>
       </c>
       <c r="D29" t="n">
-        <v>0.17119718813107</v>
+        <v>0.12971808154835</v>
       </c>
       <c r="E29" t="n">
-        <v>2.50671319700962</v>
+        <v>2.75851046599329</v>
       </c>
       <c r="F29" t="n">
-        <v>0.0121859543967516</v>
+        <v>0.00580654457885604</v>
       </c>
       <c r="G29" t="n">
-        <v>0.0307461003241118</v>
+        <v>0.0142996993359888</v>
       </c>
     </row>
     <row r="30">
@@ -1258,22 +1285,22 @@
         <v>35</v>
       </c>
       <c r="B30" t="n">
-        <v>6826.0230719088</v>
+        <v>5636.50703973795</v>
       </c>
       <c r="C30" t="n">
-        <v>0.373423318158994</v>
+        <v>0.235933122881603</v>
       </c>
       <c r="D30" t="n">
-        <v>0.125875419372011</v>
+        <v>0.0629181301951199</v>
       </c>
       <c r="E30" t="n">
-        <v>2.9666103201244</v>
+        <v>3.74984320338088</v>
       </c>
       <c r="F30" t="n">
-        <v>0.00301102316877149</v>
+        <v>0.000176945174536707</v>
       </c>
       <c r="G30" t="n">
-        <v>0.0088179964228308</v>
+        <v>0.000678975669733877</v>
       </c>
     </row>
     <row r="31">
@@ -1281,22 +1308,22 @@
         <v>36</v>
       </c>
       <c r="B31" t="n">
-        <v>8183.66414387651</v>
+        <v>7503.30920572673</v>
       </c>
       <c r="C31" t="n">
-        <v>0.397625359261421</v>
+        <v>0.92461771642745</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0929244111661489</v>
+        <v>0.191046005238553</v>
       </c>
       <c r="E31" t="n">
-        <v>4.27901941235298</v>
+        <v>4.83976472197316</v>
       </c>
       <c r="F31" t="n">
-        <v>0.0000187718492197356</v>
+        <v>0.00000129992931399238</v>
       </c>
       <c r="G31" t="n">
-        <v>0.0000993091378076333</v>
+        <v>0.00000857953347234972</v>
       </c>
     </row>
     <row r="32">
@@ -1304,22 +1331,22 @@
         <v>37</v>
       </c>
       <c r="B32" t="n">
-        <v>5583.69054531017</v>
+        <v>6691.15160148343</v>
       </c>
       <c r="C32" t="n">
-        <v>0.242644999174626</v>
+        <v>-0.652896923648559</v>
       </c>
       <c r="D32" t="n">
-        <v>0.0757208745391503</v>
+        <v>0.100742092586346</v>
       </c>
       <c r="E32" t="n">
-        <v>3.20446641235199</v>
+        <v>-6.48087514252257</v>
       </c>
       <c r="F32" t="n">
-        <v>0.00135313077275467</v>
+        <v>0.0000000000911921146224235</v>
       </c>
       <c r="G32" t="n">
-        <v>0.00435124405356404</v>
+        <v>0.00000000150466989126999</v>
       </c>
     </row>
     <row r="33">
@@ -1327,22 +1354,22 @@
         <v>38</v>
       </c>
       <c r="B33" t="n">
-        <v>7606.03497694737</v>
+        <v>5283.51300542523</v>
       </c>
       <c r="C33" t="n">
-        <v>0.740507473066003</v>
+        <v>0.864877195527324</v>
       </c>
       <c r="D33" t="n">
-        <v>0.228256656217206</v>
+        <v>0.118218880489231</v>
       </c>
       <c r="E33" t="n">
-        <v>3.24418786000854</v>
+        <v>7.31589735876505</v>
       </c>
       <c r="F33" t="n">
-        <v>0.00117786034754336</v>
+        <v>0.000000000000255667036045349</v>
       </c>
       <c r="G33" t="n">
-        <v>0.00386338193994222</v>
+        <v>0.0000000000122556166633722</v>
       </c>
     </row>
     <row r="34">
@@ -1350,22 +1377,22 @@
         <v>39</v>
       </c>
       <c r="B34" t="n">
-        <v>6393.1031419378</v>
+        <v>8315.71925219351</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.662437316998146</v>
+        <v>0.408216518832235</v>
       </c>
       <c r="D34" t="n">
-        <v>0.127189393008432</v>
+        <v>0.0900382095710964</v>
       </c>
       <c r="E34" t="n">
-        <v>-5.20827485161621</v>
+        <v>4.53381426370875</v>
       </c>
       <c r="F34" t="n">
-        <v>0.000000190604446581698</v>
+        <v>0.00000579279723848457</v>
       </c>
       <c r="G34" t="n">
-        <v>0.00000173661829107769</v>
+        <v>0.0000301783566170028</v>
       </c>
     </row>
     <row r="35">
@@ -1373,22 +1400,22 @@
         <v>40</v>
       </c>
       <c r="B35" t="n">
-        <v>5005.0761926651</v>
+        <v>2610.72893512795</v>
       </c>
       <c r="C35" t="n">
-        <v>0.960875169308764</v>
+        <v>0.825298923926777</v>
       </c>
       <c r="D35" t="n">
-        <v>0.144126319105359</v>
+        <v>0.170228105005038</v>
       </c>
       <c r="E35" t="n">
-        <v>6.66689592347356</v>
+        <v>4.84819427380898</v>
       </c>
       <c r="F35" t="n">
-        <v>0.0000000000261270228891056</v>
+        <v>0.00000124590357214426</v>
       </c>
       <c r="G35" t="n">
-        <v>0.000000000612118821973331</v>
+        <v>0.00000856558705849178</v>
       </c>
     </row>
     <row r="36">
@@ -1396,22 +1423,22 @@
         <v>41</v>
       </c>
       <c r="B36" t="n">
-        <v>7508.35003245732</v>
+        <v>4239.87946010442</v>
       </c>
       <c r="C36" t="n">
-        <v>0.501663585398554</v>
+        <v>0.962758260633185</v>
       </c>
       <c r="D36" t="n">
-        <v>0.09010502609264</v>
+        <v>0.133428433442221</v>
       </c>
       <c r="E36" t="n">
-        <v>5.56754275707969</v>
+        <v>7.21554046461989</v>
       </c>
       <c r="F36" t="n">
-        <v>0.0000000258356695407021</v>
+        <v>0.00000000000053720182682082</v>
       </c>
       <c r="G36" t="n">
-        <v>0.000000302646414619653</v>
+        <v>0.0000000000147730502375725</v>
       </c>
     </row>
     <row r="37">
@@ -1419,22 +1446,22 @@
         <v>42</v>
       </c>
       <c r="B37" t="n">
-        <v>2548.81189259703</v>
+        <v>5490.96757355454</v>
       </c>
       <c r="C37" t="n">
-        <v>1.02745201299528</v>
+        <v>-0.414576823651898</v>
       </c>
       <c r="D37" t="n">
-        <v>0.19968080291798</v>
+        <v>0.139625311898119</v>
       </c>
       <c r="E37" t="n">
-        <v>5.14547216347739</v>
+        <v>-2.96920965128733</v>
       </c>
       <c r="F37" t="n">
-        <v>0.000000266848771109694</v>
+        <v>0.00298566818143302</v>
       </c>
       <c r="G37" t="n">
-        <v>0.00000200153654124363</v>
+        <v>0.0082105874989408</v>
       </c>
     </row>
     <row r="38">
@@ -1442,22 +1469,22 @@
         <v>43</v>
       </c>
       <c r="B38" t="n">
-        <v>4364.03558925483</v>
+        <v>5727.48462080383</v>
       </c>
       <c r="C38" t="n">
-        <v>1.03390489899482</v>
+        <v>0.311653358229458</v>
       </c>
       <c r="D38" t="n">
-        <v>0.157260318517857</v>
+        <v>0.091044112714021</v>
       </c>
       <c r="E38" t="n">
-        <v>6.57448050938175</v>
+        <v>3.42310281180282</v>
       </c>
       <c r="F38" t="n">
-        <v>0.0000000000488233245893935</v>
+        <v>0.000619106561912963</v>
       </c>
       <c r="G38" t="n">
-        <v>0.000000000800702523266053</v>
+        <v>0.00201023687707711</v>
       </c>
     </row>
     <row r="39">
@@ -1465,22 +1492,22 @@
         <v>44</v>
       </c>
       <c r="B39" t="n">
-        <v>5746.64404640247</v>
+        <v>4513.92233347315</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.551578642156688</v>
+        <v>0.552383442619309</v>
       </c>
       <c r="D39" t="n">
-        <v>0.149529920840875</v>
+        <v>0.116112404948672</v>
       </c>
       <c r="E39" t="n">
-        <v>-3.68875098077301</v>
+        <v>4.75731635102633</v>
       </c>
       <c r="F39" t="n">
-        <v>0.000225357652023144</v>
+        <v>0.00000196183597310722</v>
       </c>
       <c r="G39" t="n">
-        <v>0.000879967974566563</v>
+        <v>0.0000122972617888901</v>
       </c>
     </row>
     <row r="40">
@@ -1488,22 +1515,22 @@
         <v>45</v>
       </c>
       <c r="B40" t="n">
-        <v>4325.98581686911</v>
+        <v>6138.0845041412</v>
       </c>
       <c r="C40" t="n">
-        <v>0.295713575280729</v>
+        <v>0.79114272895547</v>
       </c>
       <c r="D40" t="n">
-        <v>0.113056132266988</v>
+        <v>0.1110900656496</v>
       </c>
       <c r="E40" t="n">
-        <v>2.61563498901933</v>
+        <v>7.12163346316575</v>
       </c>
       <c r="F40" t="n">
-        <v>0.00890617091128057</v>
+        <v>0.0000000000010665538563354</v>
       </c>
       <c r="G40" t="n">
-        <v>0.023184317927778</v>
+        <v>0.0000000000219976732869175</v>
       </c>
     </row>
     <row r="41">
@@ -1511,22 +1538,22 @@
         <v>46</v>
       </c>
       <c r="B41" t="n">
-        <v>5529.26979807732</v>
+        <v>3455.48134708963</v>
       </c>
       <c r="C41" t="n">
-        <v>0.309474026936412</v>
+        <v>-0.581989006843909</v>
       </c>
       <c r="D41" t="n">
-        <v>0.112841737598512</v>
+        <v>0.131232719747215</v>
       </c>
       <c r="E41" t="n">
-        <v>2.74254928648398</v>
+        <v>-4.43478583667973</v>
       </c>
       <c r="F41" t="n">
-        <v>0.00609643001855852</v>
+        <v>0.00000921638631426906</v>
       </c>
       <c r="G41" t="n">
-        <v>0.0169460088651457</v>
+        <v>0.0000460819315713453</v>
       </c>
     </row>
     <row r="42">
@@ -1534,22 +1561,22 @@
         <v>47</v>
       </c>
       <c r="B42" t="n">
-        <v>4542.49717963328</v>
+        <v>3908.76550768387</v>
       </c>
       <c r="C42" t="n">
-        <v>0.479985411116127</v>
+        <v>-0.835382921930793</v>
       </c>
       <c r="D42" t="n">
-        <v>0.14696034469561</v>
+        <v>0.116903381447173</v>
       </c>
       <c r="E42" t="n">
-        <v>3.26608795121086</v>
+        <v>-7.14592607664039</v>
       </c>
       <c r="F42" t="n">
-        <v>0.00109044375704358</v>
+        <v>0.00000000000089391159326436</v>
       </c>
       <c r="G42" t="n">
-        <v>0.00364964849296218</v>
+        <v>0.0000000000210707732698028</v>
       </c>
     </row>
     <row r="43">
@@ -1557,22 +1584,22 @@
         <v>48</v>
       </c>
       <c r="B43" t="n">
-        <v>6026.93427764393</v>
+        <v>3567.79988832868</v>
       </c>
       <c r="C43" t="n">
-        <v>0.850535484514884</v>
+        <v>0.288994825256791</v>
       </c>
       <c r="D43" t="n">
-        <v>0.133178487298131</v>
+        <v>0.118083436095039</v>
       </c>
       <c r="E43" t="n">
-        <v>6.38643298756569</v>
+        <v>2.4473781828655</v>
       </c>
       <c r="F43" t="n">
-        <v>0.000000000169799790540007</v>
+        <v>0.0143899759817599</v>
       </c>
       <c r="G43" t="n">
-        <v>0.00000000253156051350556</v>
+        <v>0.030691744428695</v>
       </c>
     </row>
     <row r="44">
@@ -1580,22 +1607,22 @@
         <v>49</v>
       </c>
       <c r="B44" t="n">
-        <v>3663.1952121039</v>
+        <v>4232.39436341965</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.646877601874446</v>
+        <v>-0.441265168174495</v>
       </c>
       <c r="D44" t="n">
-        <v>0.135009564132902</v>
+        <v>0.116032667170182</v>
       </c>
       <c r="E44" t="n">
-        <v>-4.79134649481326</v>
+        <v>-3.80293911133924</v>
       </c>
       <c r="F44" t="n">
-        <v>0.00000165665743201273</v>
+        <v>0.000142989509081112</v>
       </c>
       <c r="G44" t="n">
-        <v>0.000010449685340388</v>
+        <v>0.000589831724959585</v>
       </c>
     </row>
     <row r="45">
@@ -1603,22 +1630,22 @@
         <v>50</v>
       </c>
       <c r="B45" t="n">
-        <v>4065.72677753591</v>
+        <v>3437.68351284455</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.919014811569757</v>
+        <v>-0.441552937647407</v>
       </c>
       <c r="D45" t="n">
-        <v>0.124044027002178</v>
+        <v>0.17225875166704</v>
       </c>
       <c r="E45" t="n">
-        <v>-7.40877923572746</v>
+        <v>-2.56331207195144</v>
       </c>
       <c r="F45" t="n">
-        <v>0.000000000000127467288413874</v>
+        <v>0.0103678811652116</v>
       </c>
       <c r="G45" t="n">
-        <v>0.0000000000069682117666251</v>
+        <v>0.0225092156876304</v>
       </c>
     </row>
     <row r="46">
@@ -1626,22 +1653,22 @@
         <v>51</v>
       </c>
       <c r="B46" t="n">
-        <v>4322.03053879335</v>
+        <v>3227.37942131371</v>
       </c>
       <c r="C46" t="n">
-        <v>-0.525130047357311</v>
+        <v>0.774646108424899</v>
       </c>
       <c r="D46" t="n">
-        <v>0.138757915793171</v>
+        <v>0.141463505724063</v>
       </c>
       <c r="E46" t="n">
-        <v>-3.78450515313345</v>
+        <v>5.47594310249822</v>
       </c>
       <c r="F46" t="n">
-        <v>0.000154014716612921</v>
+        <v>0.0000000435187516085451</v>
       </c>
       <c r="G46" t="n">
-        <v>0.000616058866451684</v>
+        <v>0.000000398921889744997</v>
       </c>
     </row>
     <row r="47">
@@ -1649,22 +1676,22 @@
         <v>52</v>
       </c>
       <c r="B47" t="n">
-        <v>3251.46400141535</v>
+        <v>4542.66379681615</v>
       </c>
       <c r="C47" t="n">
-        <v>0.944147848444847</v>
+        <v>0.931206533400246</v>
       </c>
       <c r="D47" t="n">
-        <v>0.173735284525333</v>
+        <v>0.147856668978405</v>
       </c>
       <c r="E47" t="n">
-        <v>5.43440470958089</v>
+        <v>6.29803538679916</v>
       </c>
       <c r="F47" t="n">
-        <v>0.0000000549796683136467</v>
+        <v>0.000000000301441706054781</v>
       </c>
       <c r="G47" t="n">
-        <v>0.000000601111040229204</v>
+        <v>0.00000000452162559082171</v>
       </c>
     </row>
     <row r="48">
@@ -1672,22 +1699,22 @@
         <v>53</v>
       </c>
       <c r="B48" t="n">
-        <v>4505.23195593493</v>
+        <v>2263.52306077586</v>
       </c>
       <c r="C48" t="n">
-        <v>0.991482921374952</v>
+        <v>0.520064701653626</v>
       </c>
       <c r="D48" t="n">
-        <v>0.18518600508156</v>
+        <v>0.100331333870928</v>
       </c>
       <c r="E48" t="n">
-        <v>5.35398407097923</v>
+        <v>5.18347241672944</v>
       </c>
       <c r="F48" t="n">
-        <v>0.000000086038437666477</v>
+        <v>0.000000217792451046246</v>
       </c>
       <c r="G48" t="n">
-        <v>0.000000881893986081389</v>
+        <v>0.00000165445079346617</v>
       </c>
     </row>
     <row r="49">
@@ -1695,22 +1722,22 @@
         <v>54</v>
       </c>
       <c r="B49" t="n">
-        <v>3288.73224592805</v>
+        <v>2467.32103554137</v>
       </c>
       <c r="C49" t="n">
-        <v>0.236630835836353</v>
+        <v>0.858291519526039</v>
       </c>
       <c r="D49" t="n">
-        <v>0.0984210960988094</v>
+        <v>0.102654813782375</v>
       </c>
       <c r="E49" t="n">
-        <v>2.40426946270532</v>
+        <v>8.3609476058823</v>
       </c>
       <c r="F49" t="n">
-        <v>0.0162048235789261</v>
+        <v>0.0000000000000000622164748743757</v>
       </c>
       <c r="G49" t="n">
-        <v>0.0385158125644042</v>
+        <v>0.000000000000010265718354272</v>
       </c>
     </row>
     <row r="50">
@@ -1718,22 +1745,22 @@
         <v>55</v>
       </c>
       <c r="B50" t="n">
-        <v>2299.32878157692</v>
+        <v>2749.66494359477</v>
       </c>
       <c r="C50" t="n">
-        <v>0.568496694801543</v>
+        <v>-0.290648524285897</v>
       </c>
       <c r="D50" t="n">
-        <v>0.113691588064585</v>
+        <v>0.0700126699183051</v>
       </c>
       <c r="E50" t="n">
-        <v>5.00034087375572</v>
+        <v>-4.15137038231855</v>
       </c>
       <c r="F50" t="n">
-        <v>0.000000572290439704376</v>
+        <v>0.0000330490418773241</v>
       </c>
       <c r="G50" t="n">
-        <v>0.0000039106513379799</v>
+        <v>0.000151977117842706</v>
       </c>
     </row>
     <row r="51">
@@ -1741,22 +1768,22 @@
         <v>56</v>
       </c>
       <c r="B51" t="n">
-        <v>2354.03919053216</v>
+        <v>3883.53464464444</v>
       </c>
       <c r="C51" t="n">
-        <v>0.878685429287322</v>
+        <v>0.372393598446848</v>
       </c>
       <c r="D51" t="n">
-        <v>0.11991457648687</v>
+        <v>0.114245158387188</v>
       </c>
       <c r="E51" t="n">
-        <v>7.32759481816236</v>
+        <v>3.25960070171876</v>
       </c>
       <c r="F51" t="n">
-        <v>0.000000000000234319881455019</v>
+        <v>0.00111569165556479</v>
       </c>
       <c r="G51" t="n">
-        <v>0.00000000000960711513965577</v>
+        <v>0.00340905783644798</v>
       </c>
     </row>
     <row r="52">
@@ -1764,22 +1791,22 @@
         <v>57</v>
       </c>
       <c r="B52" t="n">
-        <v>2572.99194919028</v>
+        <v>2986.77571146269</v>
       </c>
       <c r="C52" t="n">
-        <v>-0.250701150415346</v>
+        <v>-0.500215908842233</v>
       </c>
       <c r="D52" t="n">
-        <v>0.0766250760067626</v>
+        <v>0.130841751345848</v>
       </c>
       <c r="E52" t="n">
-        <v>-3.27178990847878</v>
+        <v>-3.82306032819781</v>
       </c>
       <c r="F52" t="n">
-        <v>0.00106868958232139</v>
+        <v>0.000131805514554752</v>
       </c>
       <c r="G52" t="n">
-        <v>0.00364964849296218</v>
+        <v>0.00055763871542395</v>
       </c>
     </row>
     <row r="53">
@@ -1787,22 +1814,22 @@
         <v>58</v>
       </c>
       <c r="B53" t="n">
-        <v>3369.24745345201</v>
+        <v>2828.44643300489</v>
       </c>
       <c r="C53" t="n">
-        <v>0.45262128792426</v>
+        <v>0.379021668798974</v>
       </c>
       <c r="D53" t="n">
-        <v>0.114135413687476</v>
+        <v>0.13447092826712</v>
       </c>
       <c r="E53" t="n">
-        <v>3.96565161767951</v>
+        <v>2.81861420667869</v>
       </c>
       <c r="F53" t="n">
-        <v>0.0000731957068588537</v>
+        <v>0.00482314494829589</v>
       </c>
       <c r="G53" t="n">
-        <v>0.000342974169281486</v>
+        <v>0.0128357889753036</v>
       </c>
     </row>
     <row r="54">
@@ -1810,22 +1837,22 @@
         <v>59</v>
       </c>
       <c r="B54" t="n">
-        <v>2955.08576057626</v>
+        <v>2050.23540361357</v>
       </c>
       <c r="C54" t="n">
-        <v>-0.586199487453224</v>
+        <v>-0.190101930531921</v>
       </c>
       <c r="D54" t="n">
-        <v>0.16403039417269</v>
+        <v>0.0817211155937102</v>
       </c>
       <c r="E54" t="n">
-        <v>-3.57372479905205</v>
+        <v>-2.32622779499296</v>
       </c>
       <c r="F54" t="n">
-        <v>0.000351938822926458</v>
+        <v>0.0200064016217952</v>
       </c>
       <c r="G54" t="n">
-        <v>0.00128262148799864</v>
+        <v>0.0410965009751311</v>
       </c>
     </row>
     <row r="55">
@@ -1833,22 +1860,22 @@
         <v>60</v>
       </c>
       <c r="B55" t="n">
-        <v>2907.70522473202</v>
+        <v>3244.36631776201</v>
       </c>
       <c r="C55" t="n">
-        <v>0.557258116596177</v>
+        <v>0.461921734415239</v>
       </c>
       <c r="D55" t="n">
-        <v>0.128716949991592</v>
+        <v>0.125578390727525</v>
       </c>
       <c r="E55" t="n">
-        <v>4.32932971634721</v>
+        <v>3.67835367007925</v>
       </c>
       <c r="F55" t="n">
-        <v>0.0000149563866157605</v>
+        <v>0.000234744305682343</v>
       </c>
       <c r="G55" t="n">
-        <v>0.0000817615801661574</v>
+        <v>0.000842017618208404</v>
       </c>
     </row>
     <row r="56">
@@ -1856,22 +1883,22 @@
         <v>61</v>
       </c>
       <c r="B56" t="n">
-        <v>1266.8312289158</v>
+        <v>1899.03877583482</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.618134569713431</v>
+        <v>0.25281543803426</v>
       </c>
       <c r="D56" t="n">
-        <v>0.123083738333825</v>
+        <v>0.109941272909649</v>
       </c>
       <c r="E56" t="n">
-        <v>-5.02206528726759</v>
+        <v>2.2995498536935</v>
       </c>
       <c r="F56" t="n">
-        <v>0.000000511187998335486</v>
+        <v>0.021473735871772</v>
       </c>
       <c r="G56" t="n">
-        <v>0.00000364499268378346</v>
+        <v>0.0426887520342455</v>
       </c>
     </row>
     <row r="57">
@@ -1879,22 +1906,22 @@
         <v>62</v>
       </c>
       <c r="B57" t="n">
-        <v>2001.67908809915</v>
+        <v>1194.93922681156</v>
       </c>
       <c r="C57" t="n">
-        <v>0.657366410954963</v>
+        <v>-0.535257216361659</v>
       </c>
       <c r="D57" t="n">
-        <v>0.167304862484783</v>
+        <v>0.116736824388264</v>
       </c>
       <c r="E57" t="n">
-        <v>3.92915305145272</v>
+        <v>-4.58516170168724</v>
       </c>
       <c r="F57" t="n">
-        <v>0.0000852455725148747</v>
+        <v>0.00000453635218960174</v>
       </c>
       <c r="G57" t="n">
-        <v>0.000377280930157106</v>
+        <v>0.0000258102796994582</v>
       </c>
     </row>
     <row r="58">
@@ -1902,22 +1929,22 @@
         <v>63</v>
       </c>
       <c r="B58" t="n">
-        <v>4420.48039864463</v>
+        <v>1987.40142751001</v>
       </c>
       <c r="C58" t="n">
-        <v>0.748198494069628</v>
+        <v>0.630581670088689</v>
       </c>
       <c r="D58" t="n">
-        <v>0.144810523150409</v>
+        <v>0.138534662882424</v>
       </c>
       <c r="E58" t="n">
-        <v>5.16674118560087</v>
+        <v>4.55179705186039</v>
       </c>
       <c r="F58" t="n">
-        <v>0.000000238210755948349</v>
+        <v>0.00000531896314567903</v>
       </c>
       <c r="G58" t="n">
-        <v>0.00000195332819877646</v>
+        <v>0.0000292542973012347</v>
       </c>
     </row>
     <row r="59">
@@ -1925,22 +1952,22 @@
         <v>64</v>
       </c>
       <c r="B59" t="n">
-        <v>2302.01202972758</v>
+        <v>4389.09064517735</v>
       </c>
       <c r="C59" t="n">
-        <v>1.11784605865528</v>
+        <v>0.723340549370216</v>
       </c>
       <c r="D59" t="n">
-        <v>0.164773144472494</v>
+        <v>0.124851238585258</v>
       </c>
       <c r="E59" t="n">
-        <v>6.78415200628692</v>
+        <v>5.793619331027</v>
       </c>
       <c r="F59" t="n">
-        <v>0.0000000000116770333874025</v>
+        <v>0.00000000688854991745292</v>
       </c>
       <c r="G59" t="n">
-        <v>0.000000000319172245922336</v>
+        <v>0.0000000811864811699809</v>
       </c>
     </row>
     <row r="60">
@@ -1948,22 +1975,22 @@
         <v>65</v>
       </c>
       <c r="B60" t="n">
-        <v>2984.07156144202</v>
+        <v>2412.76618268719</v>
       </c>
       <c r="C60" t="n">
-        <v>-0.448329928779044</v>
+        <v>0.976663632036001</v>
       </c>
       <c r="D60" t="n">
-        <v>0.180447927038924</v>
+        <v>0.140369046849925</v>
       </c>
       <c r="E60" t="n">
-        <v>-2.48453909189179</v>
+        <v>6.95782762620166</v>
       </c>
       <c r="F60" t="n">
-        <v>0.0129719264816482</v>
+        <v>0.00000000000345559647374128</v>
       </c>
       <c r="G60" t="n">
-        <v>0.0317521782535866</v>
+        <v>0.0000000000633526020185902</v>
       </c>
     </row>
     <row r="61">
@@ -1971,22 +1998,22 @@
         <v>66</v>
       </c>
       <c r="B61" t="n">
-        <v>1895.49368950804</v>
+        <v>1846.05250180309</v>
       </c>
       <c r="C61" t="n">
-        <v>1.1353713958136</v>
+        <v>-0.357183651945382</v>
       </c>
       <c r="D61" t="n">
-        <v>0.410551639625036</v>
+        <v>0.153754090669917</v>
       </c>
       <c r="E61" t="n">
-        <v>2.76547767986156</v>
+        <v>-2.3230838957787</v>
       </c>
       <c r="F61" t="n">
-        <v>0.00568394947133686</v>
+        <v>0.0201746459332462</v>
       </c>
       <c r="G61" t="n">
-        <v>0.0163031373110529</v>
+        <v>0.0410965009751311</v>
       </c>
     </row>
     <row r="62">
@@ -1994,22 +2021,22 @@
         <v>67</v>
       </c>
       <c r="B62" t="n">
-        <v>2199.79265486269</v>
+        <v>1994.48931302633</v>
       </c>
       <c r="C62" t="n">
-        <v>-0.608992015913912</v>
+        <v>0.935855062816348</v>
       </c>
       <c r="D62" t="n">
-        <v>0.261804600903973</v>
+        <v>0.334689130848593</v>
       </c>
       <c r="E62" t="n">
-        <v>-2.32613183195082</v>
+        <v>2.79619197804099</v>
       </c>
       <c r="F62" t="n">
-        <v>0.0200115188633056</v>
+        <v>0.00517086747638666</v>
       </c>
       <c r="G62" t="n">
-        <v>0.0455817929664183</v>
+        <v>0.0133891688386765</v>
       </c>
     </row>
     <row r="63">
@@ -2017,22 +2044,22 @@
         <v>68</v>
       </c>
       <c r="B63" t="n">
-        <v>1730.92595552647</v>
+        <v>1635.0833062071</v>
       </c>
       <c r="C63" t="n">
-        <v>-0.977565289032188</v>
+        <v>-0.81797307553221</v>
       </c>
       <c r="D63" t="n">
-        <v>0.23312517259669</v>
+        <v>0.197072850096492</v>
       </c>
       <c r="E63" t="n">
-        <v>-4.19330644624718</v>
+        <v>-4.15061270556401</v>
       </c>
       <c r="F63" t="n">
-        <v>0.0000274917655069443</v>
+        <v>0.0000331586438929541</v>
       </c>
       <c r="G63" t="n">
-        <v>0.000137053510746956</v>
+        <v>0.000151977117842706</v>
       </c>
     </row>
     <row r="64">
@@ -2040,22 +2067,22 @@
         <v>69</v>
       </c>
       <c r="B64" t="n">
-        <v>2316.40800881715</v>
+        <v>1681.30515211361</v>
       </c>
       <c r="C64" t="n">
-        <v>0.479028902492129</v>
+        <v>0.561837534930254</v>
       </c>
       <c r="D64" t="n">
-        <v>0.133012353104305</v>
+        <v>0.188085033159795</v>
       </c>
       <c r="E64" t="n">
-        <v>3.60138657284326</v>
+        <v>2.98714642782301</v>
       </c>
       <c r="F64" t="n">
-        <v>0.000316524515779514</v>
+        <v>0.0028159481240031</v>
       </c>
       <c r="G64" t="n">
-        <v>0.00117977319517818</v>
+        <v>0.00787510916034767</v>
       </c>
     </row>
     <row r="65">
@@ -2063,22 +2090,22 @@
         <v>70</v>
       </c>
       <c r="B65" t="n">
-        <v>746.352234833483</v>
+        <v>1578.56723857696</v>
       </c>
       <c r="C65" t="n">
-        <v>1.49982786202186</v>
+        <v>-0.245309823040192</v>
       </c>
       <c r="D65" t="n">
-        <v>0.62905135041478</v>
+        <v>0.105331000212731</v>
       </c>
       <c r="E65" t="n">
-        <v>2.38426936216401</v>
+        <v>-2.32894231085582</v>
       </c>
       <c r="F65" t="n">
-        <v>0.0171130712351183</v>
+        <v>0.0198621220610654</v>
       </c>
       <c r="G65" t="n">
-        <v>0.0399923968274901</v>
+        <v>0.0410965009751311</v>
       </c>
     </row>
     <row r="66">
@@ -2086,22 +2113,22 @@
         <v>71</v>
       </c>
       <c r="B66" t="n">
-        <v>171.91835390834</v>
+        <v>2164.02527766451</v>
       </c>
       <c r="C66" t="n">
-        <v>6.13237297831303</v>
+        <v>0.501059762749934</v>
       </c>
       <c r="D66" t="n">
-        <v>0.753809126261784</v>
+        <v>0.132363127955492</v>
       </c>
       <c r="E66" t="n">
-        <v>8.13518006703381</v>
+        <v>3.78549351688348</v>
       </c>
       <c r="F66" t="n">
-        <v>0.000000000000000411326510000717</v>
+        <v>0.000153403833715358</v>
       </c>
       <c r="G66" t="n">
-        <v>0.0000000000000674575476401177</v>
+        <v>0.000613136307935451</v>
       </c>
     </row>
     <row r="67">
@@ -2109,22 +2136,22 @@
         <v>72</v>
       </c>
       <c r="B67" t="n">
-        <v>753.194174246436</v>
+        <v>1170.15076776468</v>
       </c>
       <c r="C67" t="n">
-        <v>0.467207900195248</v>
+        <v>1.9053329972031</v>
       </c>
       <c r="D67" t="n">
-        <v>0.169228291670067</v>
+        <v>0.512915537621336</v>
       </c>
       <c r="E67" t="n">
-        <v>2.76081437438446</v>
+        <v>3.71471101468119</v>
       </c>
       <c r="F67" t="n">
-        <v>0.00576574368317726</v>
+        <v>0.000203436048926138</v>
       </c>
       <c r="G67" t="n">
-        <v>0.0163031373110529</v>
+        <v>0.000745932179395838</v>
       </c>
     </row>
     <row r="68">
@@ -2132,22 +2159,22 @@
         <v>73</v>
       </c>
       <c r="B68" t="n">
-        <v>740.703892787133</v>
+        <v>145.736996764115</v>
       </c>
       <c r="C68" t="n">
-        <v>0.930975867561385</v>
+        <v>6.3407359059788</v>
       </c>
       <c r="D68" t="n">
-        <v>0.405398682142628</v>
+        <v>0.773233258728883</v>
       </c>
       <c r="E68" t="n">
-        <v>2.296445224343</v>
+        <v>8.20028863787148</v>
       </c>
       <c r="F68" t="n">
-        <v>0.0216504376843712</v>
+        <v>0.000000000000000239810531218286</v>
       </c>
       <c r="G68" t="n">
-        <v>0.0479820510842821</v>
+        <v>0.0000000000000197843688255086</v>
       </c>
     </row>
     <row r="69">
@@ -2155,22 +2182,22 @@
         <v>74</v>
       </c>
       <c r="B69" t="n">
-        <v>1083.0361311981</v>
+        <v>1022.55540276679</v>
       </c>
       <c r="C69" t="n">
-        <v>1.26235533789556</v>
+        <v>0.975571214395363</v>
       </c>
       <c r="D69" t="n">
-        <v>0.204022651054345</v>
+        <v>0.349068045425528</v>
       </c>
       <c r="E69" t="n">
-        <v>6.18732935471613</v>
+        <v>2.79478808553244</v>
       </c>
       <c r="F69" t="n">
-        <v>0.000000000611920301929408</v>
+        <v>0.00519337457985027</v>
       </c>
       <c r="G69" t="n">
-        <v>0.00000000836291079303524</v>
+        <v>0.0133891688386765</v>
       </c>
     </row>
     <row r="70">
@@ -2178,22 +2205,22 @@
         <v>75</v>
       </c>
       <c r="B70" t="n">
-        <v>1087.51098832489</v>
+        <v>1221.09089632281</v>
       </c>
       <c r="C70" t="n">
-        <v>0.41652130462533</v>
+        <v>1.11596796950768</v>
       </c>
       <c r="D70" t="n">
-        <v>0.17501074122636</v>
+        <v>0.182291924081468</v>
       </c>
       <c r="E70" t="n">
-        <v>2.37997566153153</v>
+        <v>6.12187278800648</v>
       </c>
       <c r="F70" t="n">
-        <v>0.0173137815533646</v>
+        <v>0.00000000092481848492131</v>
       </c>
       <c r="G70" t="n">
-        <v>0.0399923968274901</v>
+        <v>0.000000012716254167668</v>
       </c>
     </row>
     <row r="71">
@@ -2201,22 +2228,22 @@
         <v>76</v>
       </c>
       <c r="B71" t="n">
-        <v>925.133347163617</v>
+        <v>1284.51046642438</v>
       </c>
       <c r="C71" t="n">
-        <v>0.734411694068904</v>
+        <v>1.09316713979739</v>
       </c>
       <c r="D71" t="n">
-        <v>0.149343849563675</v>
+        <v>0.475226417878574</v>
       </c>
       <c r="E71" t="n">
-        <v>4.91758914889747</v>
+        <v>2.30030801881201</v>
       </c>
       <c r="F71" t="n">
-        <v>0.000000876165591922717</v>
+        <v>0.0214307757024941</v>
       </c>
       <c r="G71" t="n">
-        <v>0.00000574764628301303</v>
+        <v>0.0426887520342455</v>
       </c>
     </row>
     <row r="72">
@@ -2224,22 +2251,22 @@
         <v>77</v>
       </c>
       <c r="B72" t="n">
-        <v>3.7373017954898</v>
+        <v>1626.80038167758</v>
       </c>
       <c r="C72" t="n">
-        <v>2.14271601345821</v>
+        <v>1.13037406957422</v>
       </c>
       <c r="D72" t="n">
-        <v>0.886992618058577</v>
+        <v>0.462431787607896</v>
       </c>
       <c r="E72" t="n">
-        <v>2.41570895837682</v>
+        <v>2.44441255957233</v>
       </c>
       <c r="F72" t="n">
-        <v>0.0157046085593352</v>
+        <v>0.0145088246390195</v>
       </c>
       <c r="G72" t="n">
-        <v>0.0378758206431026</v>
+        <v>0.030691744428695</v>
       </c>
     </row>
     <row r="73">
@@ -2247,22 +2274,22 @@
         <v>78</v>
       </c>
       <c r="B73" t="n">
-        <v>1125.30905437804</v>
+        <v>1134.26036738796</v>
       </c>
       <c r="C73" t="n">
-        <v>0.505280044292394</v>
+        <v>0.448805825280211</v>
       </c>
       <c r="D73" t="n">
-        <v>0.125761750054963</v>
+        <v>0.139595697067787</v>
       </c>
       <c r="E73" t="n">
-        <v>4.01775614661506</v>
+        <v>3.21504053998365</v>
       </c>
       <c r="F73" t="n">
-        <v>0.0000587549528048842</v>
+        <v>0.00130426101258098</v>
       </c>
       <c r="G73" t="n">
-        <v>0.000283406242941206</v>
+        <v>0.00391278303774295</v>
       </c>
     </row>
     <row r="74">
@@ -2270,22 +2297,22 @@
         <v>79</v>
       </c>
       <c r="B74" t="n">
-        <v>315.782722205069</v>
+        <v>993.919760167338</v>
       </c>
       <c r="C74" t="n">
-        <v>1.48942948070024</v>
+        <v>0.595823190014652</v>
       </c>
       <c r="D74" t="n">
-        <v>0.338323659578925</v>
+        <v>0.125378728462699</v>
       </c>
       <c r="E74" t="n">
-        <v>4.40238049728468</v>
+        <v>4.75218721166017</v>
       </c>
       <c r="F74" t="n">
-        <v>0.0000107069567006646</v>
+        <v>0.00000201227920181837</v>
       </c>
       <c r="G74" t="n">
-        <v>0.0000605496861692759</v>
+        <v>0.0000122972617888901</v>
       </c>
     </row>
     <row r="75">
@@ -2293,22 +2320,229 @@
         <v>80</v>
       </c>
       <c r="B75" t="n">
-        <v>229.238434405197</v>
+        <v>1383.93895645315</v>
       </c>
       <c r="C75" t="n">
-        <v>1.18706025375447</v>
+        <v>0.819432357185846</v>
       </c>
       <c r="D75" t="n">
-        <v>0.516537241748522</v>
+        <v>0.295598633847996</v>
       </c>
       <c r="E75" t="n">
-        <v>2.29811165161329</v>
+        <v>2.77211144895622</v>
       </c>
       <c r="F75" t="n">
-        <v>0.0215554352718635</v>
+        <v>0.00556939646959268</v>
       </c>
       <c r="G75" t="n">
-        <v>0.0479820510842821</v>
+        <v>0.0139234911739817</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>81</v>
+      </c>
+      <c r="B76" t="n">
+        <v>3.40361414293037</v>
+      </c>
+      <c r="C76" t="n">
+        <v>2.10140092699841</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.666101654802115</v>
+      </c>
+      <c r="E76" t="n">
+        <v>3.15477511855559</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.00160621859212033</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0.00473260835178314</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>82</v>
+      </c>
+      <c r="B77" t="n">
+        <v>1113.53059949069</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0.419470409272904</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0.112264096285574</v>
+      </c>
+      <c r="E77" t="n">
+        <v>3.73646092697231</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.000186628433316683</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0.00069985662493756</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>83</v>
+      </c>
+      <c r="B78" t="n">
+        <v>999.010899205259</v>
+      </c>
+      <c r="C78" t="n">
+        <v>1.89326034234371</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0.63376429691317</v>
+      </c>
+      <c r="E78" t="n">
+        <v>2.98732565334632</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.00281429764756523</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0.00787510916034767</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>84</v>
+      </c>
+      <c r="B79" t="n">
+        <v>347.45636173706</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0.451927010481832</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0.171850301777178</v>
+      </c>
+      <c r="E79" t="n">
+        <v>2.62977141039766</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.00854422985145025</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0.0197813052325579</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80" t="n">
+        <v>390.368560429129</v>
+      </c>
+      <c r="C80" t="n">
+        <v>1.4530481491578</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.280452230956936</v>
+      </c>
+      <c r="E80" t="n">
+        <v>5.18108964296641</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.000000220593439128822</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0.00000165445079346617</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>86</v>
+      </c>
+      <c r="B81" t="n">
+        <v>420.470700499657</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.22667838070254</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.0875402431799103</v>
+      </c>
+      <c r="E81" t="n">
+        <v>2.58941913419954</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0.00961379999018881</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0.0211503599784154</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82" t="n">
+        <v>204.034334902981</v>
+      </c>
+      <c r="C82" t="n">
+        <v>1.29178333843654</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0.437033369163388</v>
+      </c>
+      <c r="E82" t="n">
+        <v>2.95580024223183</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0.00311858998824446</v>
+      </c>
+      <c r="G82" t="n">
+        <v>0.00843553029607108</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>88</v>
+      </c>
+      <c r="B83" t="n">
+        <v>123.129924149095</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0.792639172797507</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0.300889269936393</v>
+      </c>
+      <c r="E83" t="n">
+        <v>2.63432183196519</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0.00843055363357141</v>
+      </c>
+      <c r="G83" t="n">
+        <v>0.0197813052325579</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>89</v>
+      </c>
+      <c r="B84" t="n">
+        <v>5.32238298226616</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0.931220328368006</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0.355210265342436</v>
+      </c>
+      <c r="E84" t="n">
+        <v>2.62160308759736</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0.00875172898167712</v>
+      </c>
+      <c r="G84" t="n">
+        <v>0.0197813052325579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>